<commit_message>
(P abängig von Q) hinzugefügt
</commit_message>
<xml_diff>
--- a/PflichtenheftTech/Ext_files/Leistungsberchnung_v2.xlsx
+++ b/PflichtenheftTech/Ext_files/Leistungsberchnung_v2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9BBA76EB-01AE-48C8-8D13-6CBD0BE8C6A4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{083974D1-93CD-4CE9-B991-445AA43E0ADE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>h in m</t>
   </si>
@@ -66,9 +66,6 @@
       </rPr>
       <t>µ:</t>
     </r>
-  </si>
-  <si>
-    <t>Zeit z [s]</t>
   </si>
   <si>
     <t>P kin in kW</t>
@@ -131,14 +128,41 @@
   <si>
     <t>Volumen Tank V [m^3]:</t>
   </si>
+  <si>
+    <t>P über Q</t>
+  </si>
+  <si>
+    <t>Querschnitsfläche A [m^2]:</t>
+  </si>
+  <si>
+    <t>Zeit z [s]:</t>
+  </si>
+  <si>
+    <t>Rohrdurchmesser d [m]:</t>
+  </si>
+  <si>
+    <r>
+      <t>A*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ρ*v^3*µ*η</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="175" formatCode="0.000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -370,7 +394,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -386,19 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -455,7 +467,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -463,17 +474,70 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -495,13 +559,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -529,26 +603,19 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,10 +631,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4D9B79C1-AB9E-47F9-B2CB-26191F0E52A6}" name="Tabelle5" displayName="Tabelle5" ref="K6:L16" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4D9B79C1-AB9E-47F9-B2CB-26191F0E52A6}" name="Tabelle5" displayName="Tabelle5" ref="K6:L22" headerRowCount="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{50141818-EC6F-4D69-928B-0B0B66167391}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="2" dataDxfId="5" totalsRowDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{74FA20B8-17BD-4BBA-81C4-F0A4F1969D94}" name="Wert" totalsRowFunction="sum" headerRowDxfId="3" dataDxfId="4" totalsRowDxfId="1" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
+    <tableColumn id="1" xr3:uid="{50141818-EC6F-4D69-928B-0B0B66167391}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="5" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{74FA20B8-17BD-4BBA-81C4-F0A4F1969D94}" name="Wert" totalsRowFunction="sum" headerRowDxfId="2" dataDxfId="1" totalsRowDxfId="0" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -836,204 +903,225 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="2.81640625" customWidth="1"/>
     <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="4" max="4" width="4.36328125" customWidth="1"/>
     <col min="5" max="5" width="20.7265625" customWidth="1"/>
     <col min="6" max="6" width="8.26953125" customWidth="1"/>
-    <col min="9" max="9" width="5.81640625" customWidth="1"/>
-    <col min="10" max="10" width="4.7265625" customWidth="1"/>
-    <col min="11" max="11" width="22.36328125" style="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" style="27" customWidth="1"/>
-    <col min="13" max="13" width="7.26953125" style="29" customWidth="1"/>
+    <col min="9" max="9" width="4.453125" customWidth="1"/>
+    <col min="10" max="10" width="3" customWidth="1"/>
+    <col min="11" max="11" width="23.26953125" style="21" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" style="23" customWidth="1"/>
+    <col min="13" max="13" width="7.26953125" style="25" customWidth="1"/>
     <col min="14" max="14" width="12.81640625" customWidth="1"/>
     <col min="15" max="15" width="14.7265625" customWidth="1"/>
+    <col min="16" max="16" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="N3" s="41" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="N3" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P3" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="30"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="26"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B5" s="20" t="s">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="18" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="16">
         <v>0.1</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="17">
         <v>0.2</v>
       </c>
-      <c r="H5" s="22">
+      <c r="H5" s="18">
         <v>0.3</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5"/>
       <c r="L5"/>
-      <c r="M5" s="30"/>
-      <c r="N5" s="36" t="s">
+      <c r="M5" s="26"/>
+      <c r="N5" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B6" s="12">
+      <c r="P5" s="31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B6" s="8">
         <v>8</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="9">
         <f>SQRT(2*9.81*B6)</f>
         <v>12.528367810692661</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="13">
         <f>(0.5*1000*F$5*C6^2)/1000</f>
         <v>7.8479999999999999</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="14">
         <f>(0.5*1000*G$5*C6^2)/1000</f>
         <v>15.696</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="15">
         <f>(0.5*1000*H$5*C6^2)/1000</f>
         <v>23.544</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="24">
         <v>9.81</v>
       </c>
-      <c r="M6" s="30"/>
-      <c r="N6" s="37">
+      <c r="M6" s="26"/>
+      <c r="N6" s="32">
         <f>O6*L12*L14</f>
         <v>64.981440000000021</v>
       </c>
-      <c r="O6" s="34">
+      <c r="O6" s="29">
         <f>(L8*L10*L6*B6)/(L16*1000)</f>
         <v>78.48</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B7" s="12">
+      <c r="P6" s="38">
+        <f>(L12*L14*L10*L20*C6^3)/(2*1000)</f>
+        <v>6.3940145056265161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B7" s="8">
         <v>10</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="9">
         <f t="shared" ref="C7:C21" si="0">SQRT(2*9.81*B7)</f>
         <v>14.007141035914502</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
-      <c r="F7" s="12">
+      <c r="F7" s="8">
         <f t="shared" ref="F7:F21" si="1">(0.5*1000*F$5*C7^2)/1000</f>
         <v>9.81</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="10">
         <f t="shared" ref="G7:G21" si="2">(0.5*1000*G$5*C7^2)/1000</f>
         <v>19.62</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="11">
         <f t="shared" ref="H7:H21" si="3">(0.5*1000*H$5*C7^2)/1000</f>
         <v>29.43</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="38">
+      <c r="K7" s="22"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="33">
         <f>O7*L12*L14</f>
         <v>81.226799999999997</v>
       </c>
-      <c r="O7" s="35">
+      <c r="O7" s="30">
         <f>(L8*L10*L6*B7)/(L16*1000)</f>
         <v>98.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B8" s="12">
+      <c r="P7" s="38">
+        <f>(L12*L14*L10*L20*C7^3)/(2*1000)</f>
+        <v>8.9359069273128746</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B8" s="8">
         <v>15</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="9">
         <f t="shared" si="0"/>
         <v>17.155174146594955</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="12">
+      <c r="F8" s="8">
         <f t="shared" si="1"/>
         <v>14.714999999999998</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="10">
         <f t="shared" si="2"/>
         <v>29.429999999999996</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="11">
         <f t="shared" si="3"/>
         <v>44.144999999999996</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" s="28">
+      <c r="K8" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="L8" s="24">
         <v>1</v>
       </c>
-      <c r="M8" s="30"/>
-      <c r="N8" s="38">
+      <c r="M8" s="26"/>
+      <c r="N8" s="33">
         <f>O8*L12*L14</f>
         <v>121.84020000000001</v>
       </c>
-      <c r="O8" s="35">
+      <c r="O8" s="30">
         <f>(L8*L10*L6*B8)/(L16*1000)</f>
         <v>147.15</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P8" s="38">
+        <f>(L12*L14*L10*L20*C8^3)/(2*1000)</f>
+        <v>16.416309270688522</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B9" s="5">
         <v>30</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="7">
         <f t="shared" si="0"/>
         <v>24.261079942986875</v>
       </c>
@@ -1053,23 +1141,27 @@
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="39">
+      <c r="K9" s="22"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="26"/>
+      <c r="N9" s="34">
         <f>O9*L12*L14</f>
         <v>243.68040000000002</v>
       </c>
-      <c r="O9" s="31">
+      <c r="O9" s="27">
         <f>(L8*L10*L6*B9)/(L16*1000)</f>
         <v>294.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P9" s="37">
+        <f>(L12*L14*L10*L20*C9^3)/(2*1000)</f>
+        <v>46.43233442943778</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B10" s="5">
         <v>40</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <f t="shared" si="0"/>
         <v>28.014282071829005</v>
       </c>
@@ -1089,27 +1181,31 @@
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="26" t="s">
-        <v>13</v>
-      </c>
-      <c r="L10" s="28">
+      <c r="K10" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="24">
         <v>1000</v>
       </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="39">
+      <c r="M10" s="26"/>
+      <c r="N10" s="34">
         <f>O10*L12*L14</f>
         <v>324.90719999999999</v>
       </c>
-      <c r="O10" s="31">
+      <c r="O10" s="27">
         <f>(L8*L10*L6*B10)/(L16*1000)</f>
         <v>392.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P10" s="37">
+        <f>(L12*L14*L10*L20*C10^3)/(2*1000)</f>
+        <v>71.487255418502997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B11" s="5">
         <v>50</v>
       </c>
-      <c r="C11" s="10">
+      <c r="C11" s="7">
         <f t="shared" si="0"/>
         <v>31.32091952673165</v>
       </c>
@@ -1129,180 +1225,200 @@
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="39">
+      <c r="K11" s="22"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="34">
         <f>O11*L12*L14</f>
         <v>406.13400000000007</v>
       </c>
-      <c r="O11" s="31">
+      <c r="O11" s="27">
         <f>(L8*L10*L6*B11)/(L16*1000)</f>
         <v>490.5</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B12" s="12">
+      <c r="P11" s="37">
+        <f>(L12*L14*L10*L20*C11^3)/(2*1000)</f>
+        <v>99.906476650414305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B12" s="8">
         <v>60</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="9">
         <f t="shared" si="0"/>
         <v>34.310348293189911</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="12">
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="8">
         <f t="shared" si="1"/>
         <v>58.859999999999992</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="10">
         <f t="shared" si="2"/>
         <v>117.71999999999998</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H12" s="11">
         <f t="shared" si="3"/>
         <v>176.57999999999998</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="28">
+      <c r="L12" s="24">
         <v>0.92</v>
       </c>
-      <c r="M12" s="30"/>
-      <c r="N12" s="38">
+      <c r="M12" s="26"/>
+      <c r="N12" s="33">
         <f>O12*L12*L14</f>
         <v>487.36080000000004</v>
       </c>
-      <c r="O12" s="35">
+      <c r="O12" s="30">
         <f>(L8*L10*L6*B12)/(L16*1000)</f>
         <v>588.6</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B13" s="12">
+      <c r="P12" s="38">
+        <f>(L12*L14*L10*L20*C12^3)/(2*1000)</f>
+        <v>131.33047416550818</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B13" s="8">
         <v>62</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="9">
         <f t="shared" si="0"/>
         <v>34.877499910400687</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="12">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="8">
         <f t="shared" si="1"/>
         <v>60.821999999999996</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="10">
         <f t="shared" si="2"/>
         <v>121.64399999999999</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="11">
         <f t="shared" si="3"/>
         <v>182.46599999999998</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="30"/>
-      <c r="N13" s="38">
+      <c r="K13" s="22"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="33">
         <f>O13*L12*L14</f>
         <v>503.60616000000005</v>
       </c>
-      <c r="O13" s="35">
+      <c r="O13" s="30">
         <f>(L8*L10*L6*B13)/(L16*1000)</f>
         <v>608.22</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B14" s="12">
+      <c r="P13" s="38">
+        <f>(L12*L14*L10*L20*C13^3)/(2*1000)</f>
+        <v>137.95141863690142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B14" s="8">
         <v>65</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="9">
         <f t="shared" si="0"/>
         <v>35.71134273588715</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="12">
+      <c r="F14" s="8">
         <f t="shared" si="1"/>
         <v>63.765000000000001</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="10">
         <f t="shared" si="2"/>
         <v>127.53</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="11">
         <f t="shared" si="3"/>
         <v>191.29499999999999</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="26" t="s">
+      <c r="K14" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="L14" s="28">
+      <c r="L14" s="24">
         <v>0.9</v>
       </c>
-      <c r="M14" s="30"/>
-      <c r="N14" s="38">
+      <c r="M14" s="26"/>
+      <c r="N14" s="33">
         <f>O14*L12*L14</f>
         <v>527.9742</v>
       </c>
-      <c r="O14" s="35">
+      <c r="O14" s="30">
         <f>(L8*L10*L6*B14)/(L16*1000)</f>
         <v>637.65</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B15" s="5">
-        <v>80</v>
-      </c>
-      <c r="C15" s="10">
+      <c r="P14" s="38">
+        <f>(L12*L14*L10*L20*C14^3)/(2*1000)</f>
+        <v>148.08418233055622</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B15" s="39">
+        <v>70</v>
+      </c>
+      <c r="C15" s="40">
         <f t="shared" si="0"/>
-        <v>39.618177646126028</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5">
+        <v>37.05941176003742</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="39">
         <f t="shared" si="1"/>
-        <v>78.48</v>
-      </c>
-      <c r="G15" s="3">
+        <v>68.67</v>
+      </c>
+      <c r="G15" s="41">
         <f t="shared" si="2"/>
-        <v>156.96</v>
-      </c>
-      <c r="H15" s="6">
+        <v>137.34</v>
+      </c>
+      <c r="H15" s="42">
         <f t="shared" si="3"/>
-        <v>235.44000000000003</v>
-      </c>
-      <c r="I15" s="1"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="30"/>
-      <c r="N15" s="39">
+        <v>206.00999999999996</v>
+      </c>
+      <c r="I15" s="53"/>
+      <c r="J15" s="54"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="56"/>
+      <c r="N15" s="43">
         <f>O15*L12*L14</f>
-        <v>649.81439999999998</v>
-      </c>
-      <c r="O15" s="31">
+        <v>568.58760000000018</v>
+      </c>
+      <c r="O15" s="44">
         <f>(L8*L10*L6*B15)/(L16*1000)</f>
-        <v>784.8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+        <v>686.7</v>
+      </c>
+      <c r="P15" s="45">
+        <f>(L12*L14*L10*L20*C15^3)/(2*1000)</f>
+        <v>165.49531227942435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B16" s="5">
         <v>100</v>
       </c>
-      <c r="C16" s="10">
+      <c r="C16" s="7">
         <f t="shared" si="0"/>
         <v>44.294469180700204</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
       <c r="F16" s="5">
         <f t="shared" si="1"/>
         <v>98.100000000000009</v>
@@ -1315,203 +1431,242 @@
         <f t="shared" si="3"/>
         <v>294.30000000000007</v>
       </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="L16" s="28">
+      <c r="I16" s="53"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="L16" s="24">
         <v>1</v>
       </c>
-      <c r="M16" s="30"/>
-      <c r="N16" s="39">
+      <c r="M16" s="56"/>
+      <c r="N16" s="34">
         <f>O16*L12*L14</f>
         <v>812.26800000000014</v>
       </c>
-      <c r="O16" s="31">
+      <c r="O16" s="27">
         <f>(L8*L10*L6*B16)/(L16*1000)</f>
         <v>981</v>
       </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B17" s="5">
-        <v>120</v>
-      </c>
-      <c r="C17" s="10">
+      <c r="P16" s="37">
+        <f>(L12*L14*L10*L20*C16^3)/(2*1000)</f>
+        <v>282.57818849585374</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B17" s="39">
+        <v>135</v>
+      </c>
+      <c r="C17" s="40">
         <f t="shared" si="0"/>
-        <v>48.52215988597375</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5">
+        <v>51.46552243978487</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="39">
         <f t="shared" si="1"/>
-        <v>117.72</v>
-      </c>
-      <c r="G17" s="3">
+        <v>132.435</v>
+      </c>
+      <c r="G17" s="41">
         <f t="shared" si="2"/>
-        <v>235.44</v>
-      </c>
-      <c r="H17" s="6">
+        <v>264.87</v>
+      </c>
+      <c r="H17" s="42">
         <f t="shared" si="3"/>
-        <v>353.16</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="30"/>
-      <c r="N17" s="39">
+        <v>397.30500000000001</v>
+      </c>
+      <c r="I17" s="53"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="56"/>
+      <c r="N17" s="43">
         <f>O17*L12*L14</f>
-        <v>974.72160000000008</v>
-      </c>
-      <c r="O17" s="31">
+        <v>1096.5618000000002</v>
+      </c>
+      <c r="O17" s="44">
         <f>(L8*L10*L6*B17)/(L16*1000)</f>
-        <v>1177.2</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B18" s="5">
-        <v>150</v>
-      </c>
-      <c r="C18" s="10">
+        <v>1324.35</v>
+      </c>
+      <c r="P17" s="45">
+        <f>(L12*L14*L10*L20*C17^3)/(2*1000)</f>
+        <v>443.24035030859017</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B18" s="39">
+        <v>205</v>
+      </c>
+      <c r="C18" s="40">
         <f t="shared" si="0"/>
-        <v>54.249423960075376</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5">
+        <v>63.420028382207462</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="39">
         <f t="shared" si="1"/>
-        <v>147.15000000000003</v>
-      </c>
-      <c r="G18" s="3">
+        <v>201.10499999999999</v>
+      </c>
+      <c r="G18" s="41">
         <f t="shared" si="2"/>
-        <v>294.30000000000007</v>
-      </c>
-      <c r="H18" s="6">
+        <v>402.21</v>
+      </c>
+      <c r="H18" s="42">
         <f t="shared" si="3"/>
-        <v>441.45000000000005</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="30"/>
-      <c r="N18" s="39">
+        <v>603.31500000000005</v>
+      </c>
+      <c r="I18" s="53"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="L18" s="60">
+        <v>0.1</v>
+      </c>
+      <c r="M18" s="56"/>
+      <c r="N18" s="43">
         <f>O18*L12*L14</f>
-        <v>1218.402</v>
-      </c>
-      <c r="O18" s="31">
+        <v>1665.1494</v>
+      </c>
+      <c r="O18" s="44">
         <f>(L8*L10*L6*B18)/(L16*1000)</f>
-        <v>1471.5</v>
-      </c>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B19" s="5">
-        <v>180</v>
-      </c>
-      <c r="C19" s="10">
+        <v>2011.05</v>
+      </c>
+      <c r="P18" s="45">
+        <f>(L12*L14*L10*L20*C18^3)/(2*1000)</f>
+        <v>829.41030755002396</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B19" s="39">
+        <v>270</v>
+      </c>
+      <c r="C19" s="40">
         <f t="shared" si="0"/>
-        <v>59.427266469189043</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="5">
+        <v>72.783239828960632</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="39">
         <f t="shared" si="1"/>
-        <v>176.58000000000004</v>
-      </c>
-      <c r="G19" s="3">
+        <v>264.87000000000006</v>
+      </c>
+      <c r="G19" s="41">
         <f t="shared" si="2"/>
-        <v>353.16000000000008</v>
-      </c>
-      <c r="H19" s="6">
+        <v>529.74000000000012</v>
+      </c>
+      <c r="H19" s="42">
         <f t="shared" si="3"/>
-        <v>529.74</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="30"/>
-      <c r="N19" s="39">
+        <v>794.61000000000024</v>
+      </c>
+      <c r="I19" s="53"/>
+      <c r="J19" s="54"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="43">
         <f>O19*L12*L14</f>
-        <v>1462.0824</v>
-      </c>
-      <c r="O19" s="31">
+        <v>2193.1236000000004</v>
+      </c>
+      <c r="O19" s="44">
         <f>(L8*L10*L6*B19)/(L16*1000)</f>
-        <v>1765.8</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
+        <v>2648.7</v>
+      </c>
+      <c r="P19" s="45">
+        <f>(L12*L14*L10*L20*C19^3)/(2*1000)</f>
+        <v>1253.6730295948203</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B20" s="5">
-        <v>250</v>
-      </c>
-      <c r="C20" s="10">
+        <v>300</v>
+      </c>
+      <c r="C20" s="7">
         <f t="shared" si="0"/>
-        <v>70.035705179572517</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+        <v>76.720271115266527</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
       <c r="F20" s="5">
         <f t="shared" si="1"/>
-        <v>245.25000000000006</v>
+        <v>294.29999999999995</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="2"/>
-        <v>490.50000000000011</v>
+        <v>588.59999999999991</v>
       </c>
       <c r="H20" s="6">
         <f t="shared" si="3"/>
-        <v>735.75000000000011</v>
-      </c>
-      <c r="I20" s="1"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="30"/>
-      <c r="N20" s="39">
+        <v>882.89999999999986</v>
+      </c>
+      <c r="I20" s="53"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="36">
+        <f>((L18)^2*3.141592)/4</f>
+        <v>7.8539800000000017E-3</v>
+      </c>
+      <c r="M20" s="56"/>
+      <c r="N20" s="34">
         <f>O20*L12*L14</f>
-        <v>2030.6700000000003</v>
-      </c>
-      <c r="O20" s="31">
+        <v>2436.8040000000001</v>
+      </c>
+      <c r="O20" s="27">
         <f>(L8*L10*L6*B20)/(L16*1000)</f>
-        <v>2452.5</v>
-      </c>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
-      <c r="B21" s="7">
-        <v>300</v>
-      </c>
-      <c r="C21" s="11">
+        <v>2943</v>
+      </c>
+      <c r="P20" s="37">
+        <f>(L12*L14*L10*L20*C20^3)/(2*1000)</f>
+        <v>1468.3193387567812</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B21" s="46">
+        <v>335</v>
+      </c>
+      <c r="C21" s="47">
         <f t="shared" si="0"/>
-        <v>76.720271115266527</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="7">
+        <v>81.07219005306321</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="46">
         <f t="shared" si="1"/>
-        <v>294.29999999999995</v>
-      </c>
-      <c r="G21" s="8">
+        <v>328.63500000000005</v>
+      </c>
+      <c r="G21" s="48">
         <f t="shared" si="2"/>
-        <v>588.59999999999991</v>
-      </c>
-      <c r="H21" s="9">
+        <v>657.2700000000001</v>
+      </c>
+      <c r="H21" s="49">
         <f t="shared" si="3"/>
-        <v>882.89999999999986</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="30"/>
-      <c r="N21" s="40">
+        <v>985.9050000000002</v>
+      </c>
+      <c r="I21" s="53"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="50">
         <f>O21*L12*L14</f>
-        <v>2436.8040000000001</v>
-      </c>
-      <c r="O21" s="32">
+        <v>2721.0978</v>
+      </c>
+      <c r="O21" s="51">
         <f>(L8*L10*L6*B21)/(L16*1000)</f>
-        <v>2943</v>
-      </c>
+        <v>3286.35</v>
+      </c>
+      <c r="P21" s="52">
+        <f>(L12*L14*L10*L20*C21^3)/(2*1000)</f>
+        <v>1732.6300695822113</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="61"/>
+      <c r="L22" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Leistung abhängig von Druck
</commit_message>
<xml_diff>
--- a/PflichtenheftTech/Ext_files/Leistungsberchnung_v2.xlsx
+++ b/PflichtenheftTech/Ext_files/Leistungsberchnung_v2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{87B32C1F-835A-4B13-8F28-0266F359C0BA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5335BACD-AF6F-40AF-B23C-1A33B689B252}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>h in m</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>Druck bar m*g/A [N/m^2]:</t>
+  </si>
+  <si>
+    <t>P über p</t>
+  </si>
+  <si>
+    <t>ρ*µ*η*g*h*A*v</t>
   </si>
 </sst>
 </file>
@@ -221,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -230,9 +236,15 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -242,30 +254,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -403,59 +391,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -472,50 +442,38 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -538,41 +496,74 @@
     <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
@@ -944,828 +935,899 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.81640625" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="2" max="2" width="8.26953125" customWidth="1"/>
     <col min="4" max="4" width="9.54296875" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
     <col min="6" max="6" width="8.26953125" customWidth="1"/>
     <col min="9" max="9" width="2.81640625" customWidth="1"/>
     <col min="10" max="10" width="2.54296875" customWidth="1"/>
-    <col min="11" max="11" width="23.26953125" style="20" customWidth="1"/>
-    <col min="12" max="12" width="10.54296875" style="22" customWidth="1"/>
-    <col min="13" max="13" width="4.54296875" style="24" customWidth="1"/>
+    <col min="11" max="11" width="23.26953125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" style="16" customWidth="1"/>
+    <col min="13" max="13" width="4.54296875" style="18" customWidth="1"/>
     <col min="14" max="14" width="12.81640625" customWidth="1"/>
     <col min="15" max="15" width="14.7265625" customWidth="1"/>
     <col min="16" max="16" width="11.90625" customWidth="1"/>
+    <col min="17" max="17" width="14.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="D3" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="D3" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="34" t="s">
+      <c r="N3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="34" t="s">
+      <c r="O3" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="34" t="s">
+      <c r="P3" s="28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="F4" s="62" t="s">
+      <c r="Q3" s="81" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="F4" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="27"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="21"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="25"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B5" s="68" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B5" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="69" t="s">
+      <c r="C5" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="16">
+      <c r="E5" s="57"/>
+      <c r="F5" s="11">
         <v>0.1</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="13">
         <v>0.2</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="12">
         <v>0.3</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5"/>
       <c r="L5"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="30" t="s">
+      <c r="M5" s="19"/>
+      <c r="N5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="27" t="s">
+      <c r="O5" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="P5" s="30" t="s">
+      <c r="P5" s="24" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B6" s="13">
+      <c r="Q5" s="76" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B6" s="9">
         <v>8</v>
       </c>
-      <c r="C6" s="70">
+      <c r="C6" s="71">
         <f>SQRT(2*9.81*B6)</f>
         <v>12.528367810692661</v>
       </c>
-      <c r="D6" s="71">
+      <c r="D6" s="59">
         <f>L6*L10*B6</f>
         <v>78480</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="13">
+      <c r="E6" s="3"/>
+      <c r="F6" s="9">
         <f>(0.5*1000*F$5*C6^2)/1000</f>
         <v>7.8479999999999999</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="65">
         <f>(0.5*1000*G$5*C6^2)/1000</f>
         <v>15.696</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="10">
         <f>(0.5*1000*H$5*C6^2)/1000</f>
         <v>23.544</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
-      <c r="K6" s="21" t="s">
+      <c r="K6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="17">
         <v>9.81</v>
       </c>
-      <c r="M6" s="25"/>
-      <c r="N6" s="31">
+      <c r="M6" s="19"/>
+      <c r="N6" s="25">
         <f>O6*L12*L14</f>
         <v>64.981440000000021</v>
       </c>
-      <c r="O6" s="28">
+      <c r="O6" s="22">
         <f>(L8*L10*L6*B6)/(L16*1000)</f>
         <v>78.48</v>
       </c>
-      <c r="P6" s="37">
+      <c r="P6" s="31">
         <f>(L12*L14*L10*L20*C6^3)/(2*1000)</f>
         <v>6.3940145056265161</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B7" s="8">
+      <c r="Q6" s="78">
+        <f>(L6*L10*L12*L14*L20*B6*C6)/(1000*L16)</f>
+        <v>6.3940145056265152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B7" s="6">
         <v>10</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="72">
         <f t="shared" ref="C7:C21" si="0">SQRT(2*9.81*B7)</f>
         <v>14.007141035914502</v>
       </c>
-      <c r="D7" s="72">
+      <c r="D7" s="60">
         <f>L6*L10*B7</f>
         <v>98100</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="8">
+      <c r="E7" s="3"/>
+      <c r="F7" s="6">
         <f t="shared" ref="F7:F21" si="1">(0.5*1000*F$5*C7^2)/1000</f>
         <v>9.81</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="66">
         <f t="shared" ref="G7:G21" si="2">(0.5*1000*G$5*C7^2)/1000</f>
         <v>19.62</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="7">
         <f t="shared" ref="H7:H21" si="3">(0.5*1000*H$5*C7^2)/1000</f>
         <v>29.43</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="32">
+      <c r="K7" s="15"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="26">
         <f>O7*L12*L14</f>
         <v>81.226799999999997</v>
       </c>
-      <c r="O7" s="29">
+      <c r="O7" s="23">
         <f>(L8*L10*L6*B7)/(L16*1000)</f>
         <v>98.1</v>
       </c>
-      <c r="P7" s="37">
+      <c r="P7" s="31">
         <f>(L12*L14*L10*L20*C7^3)/(2*1000)</f>
         <v>8.9359069273128746</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B8" s="8">
+      <c r="Q7" s="78">
+        <f>(L6*L10*L12*L14*L20*B7*C7)/(1000*L16)</f>
+        <v>8.9359069273128746</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B8" s="6">
         <v>15</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="72">
         <f t="shared" si="0"/>
         <v>17.155174146594955</v>
       </c>
-      <c r="D8" s="72">
+      <c r="D8" s="60">
         <f>L6*L10*B8</f>
         <v>147150</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="8">
+      <c r="E8" s="3"/>
+      <c r="F8" s="6">
         <f t="shared" si="1"/>
         <v>14.714999999999998</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="66">
         <f t="shared" si="2"/>
         <v>29.429999999999996</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="7">
         <f t="shared" si="3"/>
         <v>44.144999999999996</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="17">
         <v>1</v>
       </c>
-      <c r="M8" s="25"/>
-      <c r="N8" s="32">
+      <c r="M8" s="19"/>
+      <c r="N8" s="26">
         <f>O8*L12*L14</f>
         <v>121.84020000000001</v>
       </c>
-      <c r="O8" s="29">
+      <c r="O8" s="23">
         <f>(L8*L10*L6*B8)/(L16*1000)</f>
         <v>147.15</v>
       </c>
-      <c r="P8" s="37">
+      <c r="P8" s="31">
         <f>(L12*L14*L10*L20*C8^3)/(2*1000)</f>
         <v>16.416309270688522</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B9" s="5">
+      <c r="Q8" s="78">
+        <f>(L6*L10*L12*L14*L20*B8*C8)/(1000*L16)</f>
+        <v>16.416309270688526</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
         <v>30</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="73">
         <f t="shared" si="0"/>
         <v>24.261079942986875</v>
       </c>
-      <c r="D9" s="73">
+      <c r="D9" s="61">
         <f>L6*L10*B9</f>
         <v>294300</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5">
+      <c r="E9" s="3"/>
+      <c r="F9" s="4">
         <f t="shared" si="1"/>
         <v>29.43</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="67">
         <f t="shared" si="2"/>
         <v>58.86</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <f t="shared" si="3"/>
         <v>88.29</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="33">
+      <c r="K9" s="15"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="27">
         <f>O9*L12*L14</f>
         <v>243.68040000000002</v>
       </c>
-      <c r="O9" s="26">
+      <c r="O9" s="20">
         <f>(L8*L10*L6*B9)/(L16*1000)</f>
         <v>294.3</v>
       </c>
-      <c r="P9" s="36">
+      <c r="P9" s="30">
         <f>(L12*L14*L10*L20*C9^3)/(2*1000)</f>
         <v>46.43233442943778</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B10" s="5">
+      <c r="Q9" s="77">
+        <f>(L6*L10*L12*L14*L20*B9*C9)/(1000*L16)</f>
+        <v>46.432334429437773</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
         <v>40</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="73">
         <f t="shared" si="0"/>
         <v>28.014282071829005</v>
       </c>
-      <c r="D10" s="73">
+      <c r="D10" s="61">
         <f>L6*L10*B10</f>
         <v>392400</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5">
+      <c r="E10" s="3"/>
+      <c r="F10" s="4">
         <f t="shared" si="1"/>
         <v>39.24</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="67">
         <f t="shared" si="2"/>
         <v>78.48</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <f t="shared" si="3"/>
         <v>117.72</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="21" t="s">
+      <c r="K10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="17">
         <v>1000</v>
       </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="33">
+      <c r="M10" s="19"/>
+      <c r="N10" s="27">
         <f>O10*L12*L14</f>
         <v>324.90719999999999</v>
       </c>
-      <c r="O10" s="26">
+      <c r="O10" s="20">
         <f>(L8*L10*L6*B10)/(L16*1000)</f>
         <v>392.4</v>
       </c>
-      <c r="P10" s="36">
+      <c r="P10" s="30">
         <f>(L12*L14*L10*L20*C10^3)/(2*1000)</f>
         <v>71.487255418502997</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B11" s="5">
+      <c r="Q10" s="77">
+        <f>(L6*L10*L12*L14*L20*B10*C10)/(1000*L16)</f>
+        <v>71.487255418502997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
         <v>50</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="73">
         <f t="shared" si="0"/>
         <v>31.32091952673165</v>
       </c>
-      <c r="D11" s="73">
+      <c r="D11" s="61">
         <f>L6*L10*B11</f>
         <v>490500</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="5">
+      <c r="E11" s="8"/>
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
         <v>49.05</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="67">
         <f t="shared" si="2"/>
         <v>98.1</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <f t="shared" si="3"/>
         <v>147.15</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="33">
+      <c r="K11" s="15"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="27">
         <f>O11*L12*L14</f>
         <v>406.13400000000007</v>
       </c>
-      <c r="O11" s="26">
+      <c r="O11" s="20">
         <f>(L8*L10*L6*B11)/(L16*1000)</f>
         <v>490.5</v>
       </c>
-      <c r="P11" s="36">
+      <c r="P11" s="30">
         <f>(L12*L14*L10*L20*C11^3)/(2*1000)</f>
         <v>99.906476650414305</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B12" s="8">
+      <c r="Q11" s="77">
+        <f>(L6*L10*L12*L14*L20*B11*C11)/(1000*L16)</f>
+        <v>99.906476650414305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B12" s="6">
         <v>60</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="72">
         <f t="shared" si="0"/>
         <v>34.310348293189911</v>
       </c>
-      <c r="D12" s="72">
+      <c r="D12" s="60">
         <f>L6*L10*B12</f>
         <v>588600</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="8">
+      <c r="E12" s="8"/>
+      <c r="F12" s="6">
         <f t="shared" si="1"/>
         <v>58.859999999999992</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="66">
         <f t="shared" si="2"/>
         <v>117.71999999999998</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="7">
         <f t="shared" si="3"/>
         <v>176.57999999999998</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
-      <c r="K12" s="21" t="s">
+      <c r="K12" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="23">
+      <c r="L12" s="17">
         <v>0.92</v>
       </c>
-      <c r="M12" s="25"/>
-      <c r="N12" s="32">
+      <c r="M12" s="19"/>
+      <c r="N12" s="26">
         <f>O12*L12*L14</f>
         <v>487.36080000000004</v>
       </c>
-      <c r="O12" s="29">
+      <c r="O12" s="23">
         <f>(L8*L10*L6*B12)/(L16*1000)</f>
         <v>588.6</v>
       </c>
-      <c r="P12" s="37">
+      <c r="P12" s="31">
         <f>(L12*L14*L10*L20*C12^3)/(2*1000)</f>
         <v>131.33047416550818</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B13" s="8">
+      <c r="Q12" s="78">
+        <f>(L6*L10*L12*L14*L20*B12*C12)/(1000*L16)</f>
+        <v>131.33047416550821</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B13" s="6">
         <v>62</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="72">
         <f t="shared" si="0"/>
         <v>34.877499910400687</v>
       </c>
-      <c r="D13" s="72">
+      <c r="D13" s="60">
         <f>L6*L10*B13</f>
         <v>608220</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="8">
+      <c r="E13" s="3"/>
+      <c r="F13" s="6">
         <f t="shared" si="1"/>
         <v>60.821999999999996</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="66">
         <f t="shared" si="2"/>
         <v>121.64399999999999</v>
       </c>
-      <c r="H13" s="11">
+      <c r="H13" s="7">
         <f t="shared" si="3"/>
         <v>182.46599999999998</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="32">
+      <c r="K13" s="15"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="26">
         <f>O13*L12*L14</f>
         <v>503.60616000000005</v>
       </c>
-      <c r="O13" s="29">
+      <c r="O13" s="23">
         <f>(L8*L10*L6*B13)/(L16*1000)</f>
         <v>608.22</v>
       </c>
-      <c r="P13" s="37">
+      <c r="P13" s="31">
         <f>(L12*L14*L10*L20*C13^3)/(2*1000)</f>
         <v>137.95141863690142</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B14" s="8">
+      <c r="Q13" s="78">
+        <f>(L6*L10*L12*L14*L20*B13*C13)/(1000*L16)</f>
+        <v>137.95141863690145</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B14" s="6">
         <v>65</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="72">
         <f t="shared" si="0"/>
         <v>35.71134273588715</v>
       </c>
-      <c r="D14" s="72">
+      <c r="D14" s="60">
         <f>L6*L10*B14</f>
         <v>637650</v>
       </c>
-      <c r="E14" s="12"/>
-      <c r="F14" s="8">
+      <c r="E14" s="8"/>
+      <c r="F14" s="6">
         <f t="shared" si="1"/>
         <v>63.765000000000001</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="66">
         <f t="shared" si="2"/>
         <v>127.53</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="7">
         <f t="shared" si="3"/>
         <v>191.29499999999999</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="21" t="s">
+      <c r="K14" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="L14" s="23">
+      <c r="L14" s="17">
         <v>0.9</v>
       </c>
-      <c r="M14" s="25"/>
-      <c r="N14" s="32">
+      <c r="M14" s="19"/>
+      <c r="N14" s="26">
         <f>O14*L12*L14</f>
         <v>527.9742</v>
       </c>
-      <c r="O14" s="29">
+      <c r="O14" s="23">
         <f>(L8*L10*L6*B14)/(L16*1000)</f>
         <v>637.65</v>
       </c>
-      <c r="P14" s="37">
+      <c r="P14" s="31">
         <f>(L12*L14*L10*L20*C14^3)/(2*1000)</f>
         <v>148.08418233055622</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B15" s="38">
+      <c r="Q14" s="78">
+        <f>(L6*L10*L12*L14*L20*B14*C14)/(1000*L16)</f>
+        <v>148.08418233055622</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B15" s="32">
         <v>70</v>
       </c>
-      <c r="C15" s="39">
+      <c r="C15" s="74">
         <f t="shared" si="0"/>
         <v>37.05941176003742</v>
       </c>
-      <c r="D15" s="74">
+      <c r="D15" s="62">
         <f>L6*L10*B15</f>
         <v>686700</v>
       </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="38">
+      <c r="E15" s="8"/>
+      <c r="F15" s="32">
         <f t="shared" si="1"/>
         <v>68.67</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="68">
         <f t="shared" si="2"/>
         <v>137.34</v>
       </c>
-      <c r="H15" s="41">
+      <c r="H15" s="33">
         <f t="shared" si="3"/>
         <v>206.00999999999996</v>
       </c>
-      <c r="I15" s="52"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="42">
+      <c r="I15" s="42"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="46"/>
+      <c r="L15" s="47"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="34">
         <f>O15*L12*L14</f>
         <v>568.58760000000018</v>
       </c>
-      <c r="O15" s="43">
+      <c r="O15" s="35">
         <f>(L8*L10*L6*B15)/(L16*1000)</f>
         <v>686.7</v>
       </c>
-      <c r="P15" s="44">
+      <c r="P15" s="36">
         <f>(L12*L14*L10*L20*C15^3)/(2*1000)</f>
         <v>165.49531227942435</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B16" s="5">
+      <c r="Q15" s="79">
+        <f>(L6*L10*L12*L14*L20*B15*C15)/(1000*L16)</f>
+        <v>165.49531227942435</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
         <v>100</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="73">
         <f t="shared" si="0"/>
         <v>44.294469180700204</v>
       </c>
-      <c r="D16" s="75">
+      <c r="D16" s="63">
         <f>L6*L10*B16</f>
         <v>981000</v>
       </c>
-      <c r="E16" s="12"/>
-      <c r="F16" s="5">
+      <c r="E16" s="8"/>
+      <c r="F16" s="4">
         <f t="shared" si="1"/>
         <v>98.100000000000009</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="67">
         <f t="shared" si="2"/>
         <v>196.20000000000002</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <f t="shared" si="3"/>
         <v>294.30000000000007</v>
       </c>
-      <c r="I16" s="52"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="21" t="s">
+      <c r="I16" s="42"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="23">
+      <c r="L16" s="17">
         <v>1</v>
       </c>
-      <c r="M16" s="55"/>
-      <c r="N16" s="33">
+      <c r="M16" s="45"/>
+      <c r="N16" s="27">
         <f>O16*L12*L14</f>
         <v>812.26800000000014</v>
       </c>
-      <c r="O16" s="26">
+      <c r="O16" s="20">
         <f>(L8*L10*L6*B16)/(L16*1000)</f>
         <v>981</v>
       </c>
-      <c r="P16" s="36">
+      <c r="P16" s="30">
         <f>(L12*L14*L10*L20*C16^3)/(2*1000)</f>
         <v>282.57818849585374</v>
       </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B17" s="38">
+      <c r="Q16" s="77">
+        <f>(L6*L10*L12*L14*L20*B16*C16)/(1000*L16)</f>
+        <v>282.57818849585374</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B17" s="32">
         <v>135</v>
       </c>
-      <c r="C17" s="39">
+      <c r="C17" s="74">
         <f t="shared" si="0"/>
         <v>51.46552243978487</v>
       </c>
-      <c r="D17" s="74">
+      <c r="D17" s="62">
         <f>L6*L10*B17</f>
         <v>1324350</v>
       </c>
-      <c r="E17" s="12"/>
-      <c r="F17" s="38">
+      <c r="E17" s="8"/>
+      <c r="F17" s="32">
         <f t="shared" si="1"/>
         <v>132.435</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="68">
         <f t="shared" si="2"/>
         <v>264.87</v>
       </c>
-      <c r="H17" s="41">
+      <c r="H17" s="33">
         <f t="shared" si="3"/>
         <v>397.30500000000001</v>
       </c>
-      <c r="I17" s="52"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="55"/>
-      <c r="N17" s="42">
+      <c r="I17" s="42"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="46"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="34">
         <f>O17*L12*L14</f>
         <v>1096.5618000000002</v>
       </c>
-      <c r="O17" s="43">
+      <c r="O17" s="35">
         <f>(L8*L10*L6*B17)/(L16*1000)</f>
         <v>1324.35</v>
       </c>
-      <c r="P17" s="44">
+      <c r="P17" s="36">
         <f>(L12*L14*L10*L20*C17^3)/(2*1000)</f>
         <v>443.24035030859017</v>
       </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B18" s="38">
+      <c r="Q17" s="79">
+        <f>(L6*L10*L12*L14*L20*B17*C17)/(1000*L16)</f>
+        <v>443.24035030859022</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B18" s="32">
         <v>205</v>
       </c>
-      <c r="C18" s="39">
+      <c r="C18" s="74">
         <f t="shared" si="0"/>
         <v>63.420028382207462</v>
       </c>
-      <c r="D18" s="74">
+      <c r="D18" s="62">
         <f>L6*L10*B18</f>
         <v>2011050</v>
       </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="38">
+      <c r="E18" s="8"/>
+      <c r="F18" s="32">
         <f t="shared" si="1"/>
         <v>201.10499999999999</v>
       </c>
-      <c r="G18" s="40">
+      <c r="G18" s="68">
         <f t="shared" si="2"/>
         <v>402.21</v>
       </c>
-      <c r="H18" s="41">
+      <c r="H18" s="33">
         <f t="shared" si="3"/>
         <v>603.31500000000005</v>
       </c>
-      <c r="I18" s="52"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="58" t="s">
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="L18" s="59">
+      <c r="L18" s="49">
         <v>0.1</v>
       </c>
-      <c r="M18" s="55"/>
-      <c r="N18" s="42">
+      <c r="M18" s="45"/>
+      <c r="N18" s="34">
         <f>O18*L12*L14</f>
         <v>1665.1494</v>
       </c>
-      <c r="O18" s="43">
+      <c r="O18" s="35">
         <f>(L8*L10*L6*B18)/(L16*1000)</f>
         <v>2011.05</v>
       </c>
-      <c r="P18" s="44">
+      <c r="P18" s="36">
         <f>(L12*L14*L10*L20*C18^3)/(2*1000)</f>
         <v>829.41030755002396</v>
       </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B19" s="38">
+      <c r="Q18" s="79">
+        <f>(L6*L10*L12*L14*L20*B18*C18)/(1000*L16)</f>
+        <v>829.41030755002396</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B19" s="32">
         <v>270</v>
       </c>
-      <c r="C19" s="39">
+      <c r="C19" s="74">
         <f t="shared" si="0"/>
         <v>72.783239828960632</v>
       </c>
-      <c r="D19" s="74">
+      <c r="D19" s="62">
         <f>L6*L10*B19</f>
         <v>2648700</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="38">
+      <c r="E19" s="8"/>
+      <c r="F19" s="32">
         <f t="shared" si="1"/>
         <v>264.87000000000006</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="68">
         <f t="shared" si="2"/>
         <v>529.74000000000012</v>
       </c>
-      <c r="H19" s="41">
+      <c r="H19" s="33">
         <f t="shared" si="3"/>
         <v>794.61000000000024</v>
       </c>
-      <c r="I19" s="52"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="55"/>
-      <c r="N19" s="42">
+      <c r="I19" s="42"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="34">
         <f>O19*L12*L14</f>
         <v>2193.1236000000004</v>
       </c>
-      <c r="O19" s="43">
+      <c r="O19" s="35">
         <f>(L8*L10*L6*B19)/(L16*1000)</f>
         <v>2648.7</v>
       </c>
-      <c r="P19" s="44">
+      <c r="P19" s="36">
         <f>(L12*L14*L10*L20*C19^3)/(2*1000)</f>
         <v>1253.6730295948203</v>
       </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B20" s="5">
+      <c r="Q19" s="79">
+        <f>(L6*L10*L12*L14*L20*B19*C19)/(1000*L16)</f>
+        <v>1253.67302959482</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
         <v>300</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="73">
         <f t="shared" si="0"/>
         <v>76.720271115266527</v>
       </c>
-      <c r="D20" s="75">
+      <c r="D20" s="63">
         <f>L6*L10*B20</f>
         <v>2943000</v>
       </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="5">
+      <c r="E20" s="8"/>
+      <c r="F20" s="4">
         <f t="shared" si="1"/>
         <v>294.29999999999995</v>
       </c>
-      <c r="G20" s="3">
+      <c r="G20" s="67">
         <f t="shared" si="2"/>
         <v>588.59999999999991</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <f t="shared" si="3"/>
         <v>882.89999999999986</v>
       </c>
-      <c r="I20" s="52"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="21" t="s">
+      <c r="I20" s="42"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="L20" s="35">
+      <c r="L20" s="29">
         <f>((L18)^2*3.141592)/4</f>
         <v>7.8539800000000017E-3</v>
       </c>
-      <c r="M20" s="55"/>
-      <c r="N20" s="33">
+      <c r="M20" s="45"/>
+      <c r="N20" s="27">
         <f>O20*L12*L14</f>
         <v>2436.8040000000001</v>
       </c>
-      <c r="O20" s="26">
+      <c r="O20" s="20">
         <f>(L8*L10*L6*B20)/(L16*1000)</f>
         <v>2943</v>
       </c>
-      <c r="P20" s="36">
+      <c r="P20" s="30">
         <f>(L12*L14*L10*L20*C20^3)/(2*1000)</f>
         <v>1468.3193387567812</v>
       </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B21" s="45">
+      <c r="Q20" s="77">
+        <f>(L6*L10*L12*L14*L20*B20*C20)/(1000*L16)</f>
+        <v>1468.3193387567815</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="B21" s="37">
         <v>335</v>
       </c>
-      <c r="C21" s="46">
+      <c r="C21" s="75">
         <f t="shared" si="0"/>
         <v>81.07219005306321</v>
       </c>
-      <c r="D21" s="76">
+      <c r="D21" s="64">
         <f>L6*L10*B21</f>
         <v>3286350</v>
       </c>
-      <c r="F21" s="45">
+      <c r="F21" s="37">
         <f t="shared" si="1"/>
         <v>328.63500000000005</v>
       </c>
-      <c r="G21" s="47">
+      <c r="G21" s="69">
         <f t="shared" si="2"/>
         <v>657.2700000000001</v>
       </c>
-      <c r="H21" s="48">
+      <c r="H21" s="38">
         <f t="shared" si="3"/>
         <v>985.9050000000002</v>
       </c>
-      <c r="I21" s="52"/>
-      <c r="J21" s="53"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="55"/>
-      <c r="N21" s="49">
+      <c r="I21" s="42"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="45"/>
+      <c r="N21" s="39">
         <f>O21*L12*L14</f>
         <v>2721.0978</v>
       </c>
-      <c r="O21" s="50">
+      <c r="O21" s="40">
         <f>(L8*L10*L6*B21)/(L16*1000)</f>
         <v>3286.35</v>
       </c>
-      <c r="P21" s="51">
+      <c r="P21" s="41">
         <f>(L12*L14*L10*L20*C21^3)/(2*1000)</f>
         <v>1732.6300695822113</v>
       </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="F22" s="64" t="s">
+      <c r="Q21" s="80">
+        <f>(L6*L10*L12*L14*L20*B21*C21)/(1000*L16)</f>
+        <v>1732.6300695822106</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="F22" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="G22" s="65"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="60" t="s">
+      <c r="G22" s="55"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="61">
+      <c r="L22" s="51">
         <f>(L10*L8*L6)/(L20*100000)</f>
         <v>12.49048253242305</v>
       </c>

</xml_diff>

<commit_message>
Leistungsberechnung.xlsx Grobkonzept 1 berechnet
</commit_message>
<xml_diff>
--- a/PflichtenheftTech/Ext_files/Leistungsberchnung_v2.xlsx
+++ b/PflichtenheftTech/Ext_files/Leistungsberchnung_v2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5F498B64-87B9-4F9F-9AB3-E2E14EAB9A55}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2E8D0CA7-2BC6-4DA0-BA62-9BF60386AF7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="85">
   <si>
     <t>h in m</t>
   </si>
@@ -279,9 +279,6 @@
     <t>Ersparnis pro Tag [Fr]</t>
   </si>
   <si>
-    <t>Wassergeschwindigkeit [m/s]</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Dichte Wasser </t>
     </r>
@@ -347,16 +344,62 @@
   <si>
     <t>Reibungkoeffizient µ:</t>
   </si>
+  <si>
+    <t>Abstand Turbine [m]</t>
+  </si>
+  <si>
+    <t>6oben</t>
+  </si>
+  <si>
+    <t>7 mitte</t>
+  </si>
+  <si>
+    <t>9 unten</t>
+  </si>
+  <si>
+    <t>50 gesamt</t>
+  </si>
+  <si>
+    <t>Wasser pro Etage [l]</t>
+  </si>
+  <si>
+    <t>Wasser pro Block 2-6 [l]</t>
+  </si>
+  <si>
+    <t>Wasser pro Block 1 [l]</t>
+  </si>
+  <si>
+    <t>Wassergeschwindigkeit 2 Etagen [m/s]</t>
+  </si>
+  <si>
+    <t>Wassergeschwindigkeit 1 Etage [m/s]</t>
+  </si>
+  <si>
+    <t>Block 2</t>
+  </si>
+  <si>
+    <t>Block 3</t>
+  </si>
+  <si>
+    <t>Block 4</t>
+  </si>
+  <si>
+    <t>Block 5</t>
+  </si>
+  <si>
+    <t>Block 6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -386,7 +429,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,8 +478,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -632,12 +681,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -907,30 +965,26 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -940,34 +994,87 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1019,7 +1126,24 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1032,6 +1156,9 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1219,6 +1346,275 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>14942</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>14942</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>246529</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>176345</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Grafik 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A5E8DD3-809B-417B-9CB7-1BFE3716DE56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5520766" y="1695824"/>
+          <a:ext cx="3279587" cy="534933"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>29308</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>12937</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>60299</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>3871</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF758568-557F-4085-94F5-D0D23BF94BFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5529385" y="4272322"/>
+          <a:ext cx="3078991" cy="543593"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>44825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57784</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>617925</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>122769</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFF71002-9440-462F-B782-3F0C6F93BEDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5550649" y="1178372"/>
+          <a:ext cx="5199528" cy="438515"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>16745</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>32459</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>144517</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>184292</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Grafik 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7C5FB83-BF0F-444A-ADAD-8E6A68F0988F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5521538" y="2423562"/>
+          <a:ext cx="3175772" cy="519696"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>13655</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>23239</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>197069</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>178228</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Grafik 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA0085CE-35C4-4CAF-9BA8-07D94678D0F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5518448" y="3150067"/>
+          <a:ext cx="3231414" cy="522851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>7471</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>267951</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>788</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Grafik 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43D0FA5B-FBF0-4D22-B5E4-596168BA077A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5513295" y="3742765"/>
+          <a:ext cx="3308480" cy="537882"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4D9B79C1-AB9E-47F9-B2CB-26191F0E52A6}" name="Tabelle5" displayName="Tabelle5" ref="K6:L22" headerRowCount="0">
   <tableColumns count="2">
@@ -1230,10 +1626,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8C2E47EB-8D9B-4C2D-ACEE-164ABF529127}" name="Tabelle523" displayName="Tabelle523" ref="B7:C18" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1CE388F2-4887-4954-9A25-F0E8846E9A07}" name="Tabelle5234" displayName="Tabelle5234" ref="B7:C20" headerRowCount="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CC7F4B6E-63C7-441F-AA11-3850085E6C0E}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="11" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{D1A46A67-D032-44D5-AEDE-AA142025C672}" name="Wert" totalsRowFunction="sum" headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="6" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
+    <tableColumn id="1" xr3:uid="{441C20C1-2F4B-4566-B629-442D86C1BF54}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="4" dataDxfId="3" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{2D66F7F2-7825-479B-BFB1-5300857E5C8E}" name="Wert" totalsRowFunction="sum" headerRowDxfId="1" dataDxfId="0" totalsRowDxfId="2" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1242,8 +1638,8 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E660961-3964-4231-819B-2915A7872939}" name="Tabelle52" displayName="Tabelle52" ref="D7:E17" headerRowCount="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6BCF05AC-02C5-4CDB-8CD2-29F7371A94D5}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="5" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C19263DD-D321-4310-98D1-88B65D7508FA}" name="Wert" totalsRowFunction="sum" headerRowDxfId="2" dataDxfId="1" totalsRowDxfId="0" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
+    <tableColumn id="1" xr3:uid="{6BCF05AC-02C5-4CDB-8CD2-29F7371A94D5}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="11" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{C19263DD-D321-4310-98D1-88B65D7508FA}" name="Wert" totalsRowFunction="sum" headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="6" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2451,88 +2847,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAFC799-4F27-4E3F-9567-FD6C6FBCCBF7}">
-  <dimension ref="B2:L52"/>
+  <dimension ref="B2:P83"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="26.1796875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="10.54296875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" style="16" customWidth="1"/>
     <col min="4" max="4" width="9" style="18" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
-    <col min="7" max="7" width="4.90625" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" customWidth="1"/>
-    <col min="10" max="10" width="6.36328125" customWidth="1"/>
-    <col min="11" max="11" width="14.54296875" customWidth="1"/>
+    <col min="5" max="5" width="6.36328125" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" customWidth="1"/>
     <col min="12" max="12" width="11.7265625" customWidth="1"/>
+    <col min="13" max="13" width="12.6328125" customWidth="1"/>
+    <col min="14" max="14" width="12.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="E2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="18"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="E3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="18"/>
-      <c r="H3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="L3" t="s">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="N2" s="18"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E3" s="18"/>
+      <c r="N3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.35">
       <c r="D4" s="19"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N4" s="18"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="D5" s="19"/>
-      <c r="G5" s="18"/>
-      <c r="J5" s="18"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="113" t="s">
         <v>55</v>
       </c>
       <c r="C6" s="114"/>
       <c r="D6" s="19"/>
-      <c r="E6" s="90"/>
-      <c r="F6" s="117" t="s">
+      <c r="E6" s="18"/>
+      <c r="F6" s="90"/>
+      <c r="N6" s="117" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="118" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="90"/>
-      <c r="L6" s="117" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="2:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="87" t="s">
         <v>29</v>
       </c>
@@ -2540,28 +2904,22 @@
         <v>9.81</v>
       </c>
       <c r="D7" s="19"/>
-      <c r="E7" s="122" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="119">
-        <f>0.5*(C8*C10)*C11^2</f>
-        <v>56716.25</v>
-      </c>
-      <c r="G7" s="91"/>
-      <c r="H7" s="122" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="107" t="s">
-        <v>51</v>
-      </c>
-      <c r="L7" s="119">
-        <f>F$19+((C$8*C$10*12)*C$7*(C$16-(C$14*C34)))/1000000</f>
-        <v>56779.931717024003</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="E7" s="18"/>
+      <c r="F7" s="139" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="148"/>
+      <c r="H7" s="149"/>
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="149"/>
+      <c r="M7" s="150"/>
+      <c r="N7" s="137">
+        <v>2.92</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B8" s="88" t="s">
         <v>31</v>
       </c>
@@ -2569,21 +2927,18 @@
         <v>314</v>
       </c>
       <c r="D8" s="19"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="107" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" s="98">
-        <f>F$19+((C$8*C$10*12)*C$7*(C$16-(C$14*C35)))/1000000</f>
-        <v>56767.718784992001</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="E8" s="18"/>
+      <c r="F8" s="139"/>
+      <c r="G8" s="143"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="144"/>
+      <c r="N8" s="141"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9" s="88" t="s">
         <v>30</v>
       </c>
@@ -2591,21 +2946,18 @@
         <v>1000</v>
       </c>
       <c r="D9" s="19"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="91"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="107" t="s">
-        <v>49</v>
-      </c>
-      <c r="L9" s="98">
-        <f>F$19+((C$8*C$10*12)*C$7*(C$16-(C$14*C36)))/1000000</f>
-        <v>56755.505852959999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="E9" s="18"/>
+      <c r="F9" s="139"/>
+      <c r="G9" s="145"/>
+      <c r="H9" s="146"/>
+      <c r="I9" s="146"/>
+      <c r="J9" s="146"/>
+      <c r="K9" s="146"/>
+      <c r="L9" s="146"/>
+      <c r="M9" s="147"/>
+      <c r="N9" s="138"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B10" s="88" t="s">
         <v>33</v>
       </c>
@@ -2613,424 +2965,538 @@
         <v>5</v>
       </c>
       <c r="D10" s="19"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="119"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="123"/>
-      <c r="I10" s="119"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="107" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="98">
-        <f>F$19+((C$8*C$10*12)*C$7*(C$16-(C$14*C37)))/1000000</f>
-        <v>56743.292920927997</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="E10" s="18"/>
+      <c r="F10" s="140" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="148"/>
+      <c r="H10" s="149"/>
+      <c r="I10" s="149"/>
+      <c r="J10" s="149"/>
+      <c r="K10" s="149"/>
+      <c r="L10" s="149"/>
+      <c r="M10" s="150"/>
+      <c r="N10" s="137">
+        <v>7.6849999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B11" s="88" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="C11" s="89">
+        <f>C8*C10</f>
+        <v>1570</v>
+      </c>
+      <c r="E11" s="18"/>
+      <c r="F11" s="140"/>
+      <c r="G11" s="143"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="144"/>
+      <c r="N11" s="141"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B12" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="131">
+        <f>C11*12</f>
+        <v>18840</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="140"/>
+      <c r="G12" s="145"/>
+      <c r="H12" s="146"/>
+      <c r="I12" s="146"/>
+      <c r="J12" s="146"/>
+      <c r="K12" s="146"/>
+      <c r="L12" s="146"/>
+      <c r="M12" s="147"/>
+      <c r="N12" s="141"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B13" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="131">
+        <f>C11*16</f>
+        <v>25120</v>
+      </c>
+      <c r="D13" s="91"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="139" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="148"/>
+      <c r="H13" s="149"/>
+      <c r="I13" s="149"/>
+      <c r="J13" s="149"/>
+      <c r="K13" s="149"/>
+      <c r="L13" s="149"/>
+      <c r="M13" s="150"/>
+      <c r="N13" s="142">
+        <v>12.45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B14" s="132" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="130">
         <v>8.5</v>
       </c>
-      <c r="E11" s="123"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="91"/>
-      <c r="H11" s="123"/>
-      <c r="I11" s="119"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="107" t="s">
-        <v>47</v>
-      </c>
-      <c r="L11" s="98">
-        <f>F$19+((C$8*C$10*12)*C$7*(C$16-(C$14*C38)))/1000000</f>
-        <v>56731.079988896003</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="87" t="s">
+      <c r="D14" s="91"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="139"/>
+      <c r="G14" s="143"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="144"/>
+      <c r="N14" s="142"/>
+    </row>
+    <row r="15" spans="2:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B15" s="132" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="130">
+        <v>6.5</v>
+      </c>
+      <c r="D15" s="91"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="139"/>
+      <c r="G15" s="145"/>
+      <c r="H15" s="146"/>
+      <c r="I15" s="146"/>
+      <c r="J15" s="146"/>
+      <c r="K15" s="146"/>
+      <c r="L15" s="146"/>
+      <c r="M15" s="147"/>
+      <c r="N15" s="142"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B16" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="120">
+      <c r="C16" s="86">
         <v>4.72</v>
       </c>
-      <c r="D12" s="19"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="119"/>
-      <c r="G12" s="91"/>
-      <c r="H12" s="123"/>
-      <c r="I12" s="119"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="109" t="s">
-        <v>46</v>
-      </c>
-      <c r="L12" s="106">
-        <f>I23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B13" s="87" t="s">
+      <c r="D16" s="91"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="139" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="148"/>
+      <c r="H16" s="149"/>
+      <c r="I16" s="149"/>
+      <c r="J16" s="149"/>
+      <c r="K16" s="149"/>
+      <c r="L16" s="149"/>
+      <c r="M16" s="150"/>
+      <c r="N16" s="142">
+        <v>17.21</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B17" s="133" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="120">
+      <c r="C17" s="86">
         <v>0.8</v>
       </c>
-      <c r="D13" s="91"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="119"/>
-      <c r="G13" s="91"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="119"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="108" t="s">
-        <v>52</v>
-      </c>
-      <c r="L13" s="98">
-        <f>L7+L8+L9+L10+L11+L12</f>
-        <v>283777.52926480002</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B14" s="88" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="121">
-        <v>66.08</v>
-      </c>
-      <c r="D14" s="91"/>
-      <c r="E14" s="123"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="91"/>
-      <c r="H14" s="123"/>
-      <c r="I14" s="119"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="125" t="s">
-        <v>54</v>
-      </c>
-      <c r="L14" s="126">
-        <f>L13*C13</f>
-        <v>227022.02341184003</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B15" s="87" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="120">
-        <v>80.239999999999995</v>
-      </c>
-      <c r="D15" s="91"/>
-      <c r="E15" s="123"/>
-      <c r="F15" s="119"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="123"/>
-      <c r="I15" s="119"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="125"/>
-      <c r="L15" s="126"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B16" s="87" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="120">
-        <f>C15+(5*C14)</f>
-        <v>410.64</v>
-      </c>
-      <c r="D16" s="91"/>
-      <c r="E16" s="123"/>
-      <c r="F16" s="119"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="123"/>
-      <c r="I16" s="119"/>
-      <c r="J16" s="18"/>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B17" s="88" t="s">
+      <c r="D17" s="91"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="143"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="144"/>
+      <c r="N17" s="142"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B18" s="134" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="85">
+        <v>9.44</v>
+      </c>
+      <c r="D18" s="91"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="139"/>
+      <c r="G18" s="145"/>
+      <c r="H18" s="146"/>
+      <c r="I18" s="146"/>
+      <c r="J18" s="146"/>
+      <c r="K18" s="146"/>
+      <c r="L18" s="146"/>
+      <c r="M18" s="147"/>
+      <c r="N18" s="142"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B19" s="134" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="121">
+      <c r="C19" s="85">
         <v>0.2</v>
       </c>
-      <c r="D17" s="91"/>
-      <c r="E17" s="123"/>
-      <c r="F17" s="119"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="123"/>
-      <c r="I17" s="119"/>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="115"/>
-      <c r="C18" s="116"/>
-      <c r="D18" s="91"/>
-      <c r="E18" s="124"/>
-      <c r="F18" s="119"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="123"/>
-      <c r="I18" s="119"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="127" t="s">
-        <v>56</v>
-      </c>
-      <c r="L18" s="128">
-        <f>(L14*1000000)/3600000</f>
-        <v>63061.67316995556</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B19" s="111"/>
-      <c r="C19" s="112"/>
       <c r="D19" s="91"/>
-      <c r="E19" s="98" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="105">
-        <f>F7+F8+F9+F10+F11+F12+F13+F14+F15+F16+F17+F18</f>
-        <v>56716.25</v>
-      </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="123"/>
-      <c r="I19" s="119"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="127"/>
-      <c r="L19" s="128"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="111"/>
-      <c r="C20" s="112"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="139" t="s">
+        <v>80</v>
+      </c>
+      <c r="G19" s="148"/>
+      <c r="H19" s="149"/>
+      <c r="I19" s="149"/>
+      <c r="J19" s="149"/>
+      <c r="K19" s="149"/>
+      <c r="L19" s="149"/>
+      <c r="M19" s="150"/>
+      <c r="N19" s="142">
+        <v>21.98</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="115"/>
+      <c r="C20" s="116"/>
       <c r="D20" s="91"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="123"/>
-      <c r="I20" s="119"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="129" t="s">
-        <v>58</v>
-      </c>
-      <c r="L20" s="128">
-        <f>L18*C17</f>
-        <v>12612.334633991113</v>
-      </c>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="111"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="139"/>
+      <c r="G20" s="143"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="144"/>
+      <c r="N20" s="142"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B21" s="159"/>
       <c r="C21" s="112"/>
       <c r="D21" s="91"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="123"/>
-      <c r="I21" s="119"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="129"/>
-      <c r="L21" s="128"/>
-    </row>
-    <row r="22" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E21" s="18"/>
+      <c r="F21" s="139"/>
+      <c r="G21" s="145"/>
+      <c r="H21" s="146"/>
+      <c r="I21" s="146"/>
+      <c r="J21" s="146"/>
+      <c r="K21" s="146"/>
+      <c r="L21" s="146"/>
+      <c r="M21" s="147"/>
+      <c r="N21" s="142"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B22" s="103"/>
       <c r="C22" s="104"/>
       <c r="D22" s="91"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="96"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="124"/>
-      <c r="I22" s="119"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="96"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="F22" s="139" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="148"/>
+      <c r="H22" s="149"/>
+      <c r="I22" s="149"/>
+      <c r="J22" s="149"/>
+      <c r="K22" s="149"/>
+      <c r="L22" s="149"/>
+      <c r="M22" s="150"/>
+      <c r="N22" s="142">
+        <v>34.520000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.35">
       <c r="D23" s="91"/>
-      <c r="F23" s="95"/>
-      <c r="H23" s="98" t="s">
-        <v>36</v>
-      </c>
-      <c r="I23" s="105">
-        <f>I7+I8+I9+I10+I11+I12+I13+I14+I15+I16+I17+I18+I19+I20+I21+I22</f>
-        <v>0</v>
-      </c>
-      <c r="L23" s="95"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="F23" s="139"/>
+      <c r="G23" s="143"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="144"/>
+      <c r="N23" s="142"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.35">
       <c r="D24" s="91"/>
-      <c r="F24" s="95"/>
-      <c r="I24" s="101"/>
-      <c r="L24" s="95"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="F25" s="95"/>
-      <c r="I25" s="101"/>
-      <c r="L25" s="95"/>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="F26" s="95"/>
-      <c r="I26" s="95"/>
-      <c r="L26" s="110"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="F24" s="139"/>
+      <c r="G24" s="145"/>
+      <c r="H24" s="146"/>
+      <c r="I24" s="146"/>
+      <c r="J24" s="146"/>
+      <c r="K24" s="146"/>
+      <c r="L24" s="146"/>
+      <c r="M24" s="147"/>
+      <c r="N24" s="142"/>
+      <c r="P24" s="2"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="M25" s="151" t="s">
+        <v>52</v>
+      </c>
+      <c r="N25" s="152">
+        <f>N7+N10+N13+N16+N19+N22</f>
+        <v>96.765000000000015</v>
+      </c>
+      <c r="P25" s="101"/>
+    </row>
+    <row r="26" spans="2:16" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M26" s="119" t="s">
+        <v>54</v>
+      </c>
+      <c r="N26" s="153">
+        <f>N25*C17</f>
+        <v>77.41200000000002</v>
+      </c>
+      <c r="P26" s="158"/>
+    </row>
+    <row r="27" spans="2:16" ht="9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="103"/>
-      <c r="C27" s="104"/>
-      <c r="F27" s="95"/>
-      <c r="I27" s="95"/>
-      <c r="L27" s="95"/>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="F27" s="160"/>
+      <c r="P27" s="158"/>
+    </row>
+    <row r="28" spans="2:16" ht="5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="103"/>
       <c r="C28" s="104"/>
-      <c r="F28" s="95"/>
-      <c r="I28" s="95"/>
-      <c r="L28" s="95"/>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="N28" s="95"/>
+      <c r="P28" s="2"/>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B29" s="103"/>
       <c r="C29" s="104"/>
-      <c r="F29" s="95"/>
-      <c r="I29" s="95"/>
-      <c r="L29" s="95"/>
-    </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="M29" s="154" t="s">
+        <v>56</v>
+      </c>
+      <c r="N29" s="135">
+        <f>(N26*1000000)/3600000</f>
+        <v>21.503333333333337</v>
+      </c>
+      <c r="P29" s="2"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B30" s="103"/>
       <c r="C30" s="104"/>
-      <c r="F30" s="95"/>
-      <c r="I30" s="95"/>
-      <c r="L30" s="95"/>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="M30" s="155"/>
+      <c r="N30" s="136"/>
+    </row>
+    <row r="31" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="103"/>
       <c r="C31" s="104"/>
-      <c r="F31" s="95"/>
-      <c r="H31" s="91"/>
-      <c r="I31" s="101"/>
-      <c r="L31" s="95"/>
-    </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="F32" s="95"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="99"/>
-      <c r="L32" s="95"/>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C33">
-        <v>0</v>
-      </c>
-      <c r="F33" s="95"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="99"/>
-      <c r="L33" s="95"/>
-    </row>
-    <row r="34" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="F34" s="95"/>
-      <c r="I34" s="95"/>
-      <c r="L34" s="95"/>
-    </row>
-    <row r="35" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="F35" s="95"/>
-      <c r="I35" s="95"/>
-      <c r="L35" s="95"/>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C40">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C41">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C42">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C43">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C44">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C45">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C46">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C47">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="C48">
-        <v>15</v>
-      </c>
+      <c r="M31" s="156" t="s">
+        <v>58</v>
+      </c>
+      <c r="N31" s="135">
+        <f>N29*C19</f>
+        <v>4.3006666666666673</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="M32" s="157"/>
+      <c r="N32" s="136"/>
+    </row>
+    <row r="33" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C33"/>
+      <c r="N33" s="95"/>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C34"/>
+      <c r="N34" s="95"/>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C35"/>
+      <c r="N35" s="95"/>
+    </row>
+    <row r="36" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C36"/>
+    </row>
+    <row r="37" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C37"/>
+    </row>
+    <row r="38" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C38"/>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C39"/>
+      <c r="E39" s="16"/>
+    </row>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C40"/>
+      <c r="E40" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C41"/>
+      <c r="E41" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C42"/>
+      <c r="E42" s="16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C43"/>
+      <c r="E43" s="104" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="44" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C44"/>
+    </row>
+    <row r="45" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C45"/>
+    </row>
+    <row r="46" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C46"/>
+    </row>
+    <row r="47" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C47"/>
+    </row>
+    <row r="48" spans="3:14" x14ac:dyDescent="0.35">
+      <c r="C48"/>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C49">
-        <v>16</v>
-      </c>
+      <c r="C49"/>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C50">
-        <v>17</v>
-      </c>
+      <c r="C50"/>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.35">
-      <c r="C51">
-        <v>18</v>
-      </c>
+      <c r="C51"/>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C52"/>
       <c r="D52"/>
     </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C53"/>
+    </row>
+    <row r="54" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C54"/>
+    </row>
+    <row r="55" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C55"/>
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C56"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C57"/>
+    </row>
+    <row r="58" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C58"/>
+    </row>
+    <row r="59" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C59"/>
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C60"/>
+    </row>
+    <row r="61" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C61"/>
+    </row>
+    <row r="62" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C62"/>
+    </row>
+    <row r="63" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C63"/>
+    </row>
+    <row r="64" spans="3:4" x14ac:dyDescent="0.35">
+      <c r="C64"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C65"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C66"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C67"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C68"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C69"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C70"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C71"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C72"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C73"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C74"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C75"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C76"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C77"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C78"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C79"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C80"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C81"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C82"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C83"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="E7:E18"/>
-    <mergeCell ref="H7:H22"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
+  <mergeCells count="16">
+    <mergeCell ref="M29:M30"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="N29:N30"/>
+    <mergeCell ref="N31:N32"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="N7:N9"/>
+    <mergeCell ref="N10:N12"/>
+    <mergeCell ref="N13:N15"/>
+    <mergeCell ref="N16:N18"/>
+    <mergeCell ref="N19:N21"/>
+    <mergeCell ref="N22:N24"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F10:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3049,11 +3515,11 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="120" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="120" t="s">
         <v>66</v>
-      </c>
-      <c r="C6" s="130" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -3066,7 +3532,7 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8">
         <v>1000</v>
@@ -3074,7 +3540,7 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9">
         <v>1.57</v>
@@ -3082,7 +3548,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>4.72</v>
@@ -3090,7 +3556,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11">
         <v>0.8</v>
@@ -3098,7 +3564,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C12">
         <v>0.9</v>
@@ -3114,9 +3580,9 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="131">
+        <v>64</v>
+      </c>
+      <c r="C14" s="121">
         <v>86400</v>
       </c>
     </row>
@@ -3130,8 +3596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40C3B2D-E4BE-4431-A41F-5268AC320356}">
   <dimension ref="B6:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3140,11 +3606,11 @@
   </cols>
   <sheetData>
     <row r="6" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="120" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="120" t="s">
         <v>66</v>
-      </c>
-      <c r="C6" s="130" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.35">
@@ -3157,7 +3623,7 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8">
         <v>1000</v>
@@ -3165,7 +3631,7 @@
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9">
         <v>1.57</v>
@@ -3173,7 +3639,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>4.72</v>
@@ -3181,7 +3647,7 @@
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>0.8</v>
@@ -3189,7 +3655,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12">
         <v>0.9</v>
@@ -3205,9 +3671,9 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="131">
+        <v>64</v>
+      </c>
+      <c r="C14" s="121">
         <v>86400</v>
       </c>
     </row>
@@ -3221,7 +3687,7 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="N20" sqref="N20:N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Leistungsberechnung.xlsx Alle Grobkonzepte berechnet
</commit_message>
<xml_diff>
--- a/PflichtenheftTech/Ext_files/Leistungsberchnung_v2.xlsx
+++ b/PflichtenheftTech/Ext_files/Leistungsberchnung_v2.xlsx
@@ -3,16 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DF37F071-FEE9-466C-8653-FAA716702742}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AF169FF9-DA49-4FE4-8268-2EA380C6F6CF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Grobkonzept 1" sheetId="3" r:id="rId2"/>
-    <sheet name="Grobkonzept 2" sheetId="5" r:id="rId3"/>
-    <sheet name="Grobkonzept3" sheetId="4" r:id="rId4"/>
+    <sheet name="Grobkonzept 2" sheetId="6" r:id="rId3"/>
+    <sheet name="Grobkonzept 3" sheetId="7" r:id="rId4"/>
     <sheet name="Grobkonzept 4" sheetId="2" r:id="rId5"/>
+    <sheet name="Grobkonzept 3 misch" sheetId="4" r:id="rId6"/>
+    <sheet name="Grobkonzept 2 misch" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="112">
   <si>
     <t>h in m</t>
   </si>
@@ -479,6 +481,18 @@
   </si>
   <si>
     <t>E=(12*V*ρ*g*65m*(1+η)^4)/10EE6</t>
+  </si>
+  <si>
+    <t>v= Wurzel(2 *g * h)</t>
+  </si>
+  <si>
+    <t>Benutze Etagen Block 1</t>
+  </si>
+  <si>
+    <t>Benutze Etagen pro Block 2-6</t>
+  </si>
+  <si>
+    <t>E = 0.5 * m * v^2</t>
   </si>
 </sst>
 </file>
@@ -786,7 +800,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1101,10 +1115,37 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1116,27 +1157,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1159,6 +1179,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1166,7 +1201,177 @@
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="35" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1710,8 +1915,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4D9B79C1-AB9E-47F9-B2CB-26191F0E52A6}" name="Tabelle5" displayName="Tabelle5" ref="K6:L22" headerRowCount="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{50141818-EC6F-4D69-928B-0B0B66167391}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{74FA20B8-17BD-4BBA-81C4-F0A4F1969D94}" name="Wert" totalsRowFunction="sum" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
+    <tableColumn id="1" xr3:uid="{50141818-EC6F-4D69-928B-0B0B66167391}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="29" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{74FA20B8-17BD-4BBA-81C4-F0A4F1969D94}" name="Wert" totalsRowFunction="sum" headerRowDxfId="26" dataDxfId="25" totalsRowDxfId="24" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1720,18 +1925,38 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1CE388F2-4887-4954-9A25-F0E8846E9A07}" name="Tabelle5234" displayName="Tabelle5234" ref="B7:C20" headerRowCount="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{441C20C1-2F4B-4566-B629-442D86C1BF54}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="11" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{2D66F7F2-7825-479B-BFB1-5300857E5C8E}" name="Wert" totalsRowFunction="sum" headerRowDxfId="8" dataDxfId="7" totalsRowDxfId="6" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
+    <tableColumn id="1" xr3:uid="{441C20C1-2F4B-4566-B629-442D86C1BF54}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="23" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{2D66F7F2-7825-479B-BFB1-5300857E5C8E}" name="Wert" totalsRowFunction="sum" headerRowDxfId="20" dataDxfId="19" totalsRowDxfId="18" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9E43B6E6-9D26-4EED-99FC-7BC708784230}" name="Tabelle52343" displayName="Tabelle52343" ref="B7:C20" headerRowCount="0">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{17CD5B59-FCCA-490E-BC34-1156D8F61388}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{9EA22398-EF4F-4CD4-9E4C-372521DC2965}" name="Wert" totalsRowFunction="sum" headerRowDxfId="7" dataDxfId="6" totalsRowDxfId="8" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1B0065A7-448C-41A6-B927-B964CA642EBC}" name="Tabelle523435" displayName="Tabelle523435" ref="B7:C20" headerRowCount="0">
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{668B213C-821C-4C11-B51D-1204217E3F92}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="4" dataDxfId="3" totalsRowDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{7137C260-F60F-472B-884D-26B5E16880DE}" name="Wert" totalsRowFunction="sum" headerRowDxfId="1" dataDxfId="0" totalsRowDxfId="2" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7E660961-3964-4231-819B-2915A7872939}" name="Tabelle52" displayName="Tabelle52" ref="D7:E17" headerRowCount="0">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6BCF05AC-02C5-4CDB-8CD2-29F7371A94D5}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="5" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{C19263DD-D321-4310-98D1-88B65D7508FA}" name="Wert" totalsRowFunction="sum" headerRowDxfId="2" dataDxfId="1" totalsRowDxfId="0" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
+    <tableColumn id="1" xr3:uid="{6BCF05AC-02C5-4CDB-8CD2-29F7371A94D5}" name="Einheit" totalsRowLabel="Ergebnis" headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C19263DD-D321-4310-98D1-88B65D7508FA}" name="Wert" totalsRowFunction="sum" headerRowDxfId="14" dataDxfId="13" totalsRowDxfId="12" headerRowCellStyle="Komma" dataCellStyle="Komma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2002,7 +2227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
@@ -2941,8 +3166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEAFC799-4F27-4E3F-9567-FD6C6FBCCBF7}">
   <dimension ref="B2:P83"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2997,7 +3222,7 @@
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="18"/>
-      <c r="F7" s="142" t="s">
+      <c r="F7" s="144" t="s">
         <v>84</v>
       </c>
       <c r="G7" s="132"/>
@@ -3007,7 +3232,7 @@
       <c r="K7" s="133"/>
       <c r="L7" s="133"/>
       <c r="M7" s="134"/>
-      <c r="N7" s="144">
+      <c r="N7" s="153">
         <v>2.92</v>
       </c>
     </row>
@@ -3020,7 +3245,7 @@
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="18"/>
-      <c r="F8" s="142"/>
+      <c r="F8" s="144"/>
       <c r="G8" s="127"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -3028,7 +3253,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="128"/>
-      <c r="N8" s="145"/>
+      <c r="N8" s="154"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B9" s="88" t="s">
@@ -3039,7 +3264,7 @@
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="18"/>
-      <c r="F9" s="142"/>
+      <c r="F9" s="144"/>
       <c r="G9" s="129"/>
       <c r="H9" s="130"/>
       <c r="I9" s="130"/>
@@ -3047,7 +3272,7 @@
       <c r="K9" s="130"/>
       <c r="L9" s="130"/>
       <c r="M9" s="131"/>
-      <c r="N9" s="146"/>
+      <c r="N9" s="155"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B10" s="88" t="s">
@@ -3058,7 +3283,7 @@
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="143" t="s">
+      <c r="F10" s="152" t="s">
         <v>83</v>
       </c>
       <c r="G10" s="132"/>
@@ -3068,7 +3293,7 @@
       <c r="K10" s="133"/>
       <c r="L10" s="133"/>
       <c r="M10" s="134"/>
-      <c r="N10" s="144">
+      <c r="N10" s="153">
         <v>7.6849999999999996</v>
       </c>
     </row>
@@ -3081,7 +3306,7 @@
         <v>1570</v>
       </c>
       <c r="E11" s="18"/>
-      <c r="F11" s="143"/>
+      <c r="F11" s="152"/>
       <c r="G11" s="127"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -3089,7 +3314,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="128"/>
-      <c r="N11" s="145"/>
+      <c r="N11" s="154"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B12" s="87" t="s">
@@ -3101,7 +3326,7 @@
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="18"/>
-      <c r="F12" s="143"/>
+      <c r="F12" s="152"/>
       <c r="G12" s="129"/>
       <c r="H12" s="130"/>
       <c r="I12" s="130"/>
@@ -3109,7 +3334,7 @@
       <c r="K12" s="130"/>
       <c r="L12" s="130"/>
       <c r="M12" s="131"/>
-      <c r="N12" s="145"/>
+      <c r="N12" s="154"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B13" s="87" t="s">
@@ -3121,7 +3346,7 @@
       </c>
       <c r="D13" s="91"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="142" t="s">
+      <c r="F13" s="144" t="s">
         <v>82</v>
       </c>
       <c r="G13" s="132"/>
@@ -3131,7 +3356,7 @@
       <c r="K13" s="133"/>
       <c r="L13" s="133"/>
       <c r="M13" s="134"/>
-      <c r="N13" s="147">
+      <c r="N13" s="145">
         <v>12.45</v>
       </c>
     </row>
@@ -3144,7 +3369,7 @@
       </c>
       <c r="D14" s="91"/>
       <c r="E14" s="18"/>
-      <c r="F14" s="142"/>
+      <c r="F14" s="144"/>
       <c r="G14" s="127"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -3152,7 +3377,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="128"/>
-      <c r="N14" s="147"/>
+      <c r="N14" s="145"/>
     </row>
     <row r="15" spans="2:14" ht="29" x14ac:dyDescent="0.35">
       <c r="B15" s="124" t="s">
@@ -3163,7 +3388,7 @@
       </c>
       <c r="D15" s="91"/>
       <c r="E15" s="18"/>
-      <c r="F15" s="142"/>
+      <c r="F15" s="144"/>
       <c r="G15" s="129"/>
       <c r="H15" s="130"/>
       <c r="I15" s="130"/>
@@ -3171,7 +3396,7 @@
       <c r="K15" s="130"/>
       <c r="L15" s="130"/>
       <c r="M15" s="131"/>
-      <c r="N15" s="147"/>
+      <c r="N15" s="145"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B16" s="125" t="s">
@@ -3182,7 +3407,7 @@
       </c>
       <c r="D16" s="91"/>
       <c r="E16" s="18"/>
-      <c r="F16" s="142" t="s">
+      <c r="F16" s="144" t="s">
         <v>81</v>
       </c>
       <c r="G16" s="132"/>
@@ -3192,7 +3417,7 @@
       <c r="K16" s="133"/>
       <c r="L16" s="133"/>
       <c r="M16" s="134"/>
-      <c r="N16" s="147">
+      <c r="N16" s="145">
         <v>17.21</v>
       </c>
     </row>
@@ -3205,7 +3430,7 @@
       </c>
       <c r="D17" s="91"/>
       <c r="E17" s="18"/>
-      <c r="F17" s="142"/>
+      <c r="F17" s="144"/>
       <c r="G17" s="127"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -3213,7 +3438,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="128"/>
-      <c r="N17" s="147"/>
+      <c r="N17" s="145"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B18" s="126" t="s">
@@ -3224,7 +3449,7 @@
       </c>
       <c r="D18" s="91"/>
       <c r="E18" s="18"/>
-      <c r="F18" s="142"/>
+      <c r="F18" s="144"/>
       <c r="G18" s="129"/>
       <c r="H18" s="130"/>
       <c r="I18" s="130"/>
@@ -3232,7 +3457,7 @@
       <c r="K18" s="130"/>
       <c r="L18" s="130"/>
       <c r="M18" s="131"/>
-      <c r="N18" s="147"/>
+      <c r="N18" s="145"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" s="126" t="s">
@@ -3243,7 +3468,7 @@
       </c>
       <c r="D19" s="91"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="142" t="s">
+      <c r="F19" s="144" t="s">
         <v>80</v>
       </c>
       <c r="G19" s="132"/>
@@ -3253,7 +3478,7 @@
       <c r="K19" s="133"/>
       <c r="L19" s="133"/>
       <c r="M19" s="134"/>
-      <c r="N19" s="147">
+      <c r="N19" s="145">
         <v>21.98</v>
       </c>
     </row>
@@ -3262,7 +3487,7 @@
       <c r="C20" s="116"/>
       <c r="D20" s="91"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="142"/>
+      <c r="F20" s="144"/>
       <c r="G20" s="127"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -3270,14 +3495,14 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="128"/>
-      <c r="N20" s="147"/>
+      <c r="N20" s="145"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="139"/>
       <c r="C21" s="112"/>
       <c r="D21" s="91"/>
       <c r="E21" s="18"/>
-      <c r="F21" s="142"/>
+      <c r="F21" s="144"/>
       <c r="G21" s="129"/>
       <c r="H21" s="130"/>
       <c r="I21" s="130"/>
@@ -3285,14 +3510,14 @@
       <c r="K21" s="130"/>
       <c r="L21" s="130"/>
       <c r="M21" s="131"/>
-      <c r="N21" s="147"/>
+      <c r="N21" s="145"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B22" s="103"/>
       <c r="C22" s="104"/>
       <c r="D22" s="91"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="142" t="s">
+      <c r="F22" s="144" t="s">
         <v>36</v>
       </c>
       <c r="G22" s="132"/>
@@ -3302,13 +3527,13 @@
       <c r="K22" s="133"/>
       <c r="L22" s="133"/>
       <c r="M22" s="134"/>
-      <c r="N22" s="147">
+      <c r="N22" s="145">
         <v>34.520000000000003</v>
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.35">
       <c r="D23" s="91"/>
-      <c r="F23" s="142"/>
+      <c r="F23" s="144"/>
       <c r="G23" s="127"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
@@ -3316,11 +3541,11 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
       <c r="M23" s="128"/>
-      <c r="N23" s="147"/>
+      <c r="N23" s="145"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.35">
       <c r="D24" s="91"/>
-      <c r="F24" s="142"/>
+      <c r="F24" s="144"/>
       <c r="G24" s="129"/>
       <c r="H24" s="130"/>
       <c r="I24" s="130"/>
@@ -3328,7 +3553,7 @@
       <c r="K24" s="130"/>
       <c r="L24" s="130"/>
       <c r="M24" s="131"/>
-      <c r="N24" s="147"/>
+      <c r="N24" s="145"/>
       <c r="P24" s="2"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.35">
@@ -3365,10 +3590,10 @@
     <row r="29" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B29" s="103"/>
       <c r="C29" s="104"/>
-      <c r="M29" s="148" t="s">
+      <c r="M29" s="146" t="s">
         <v>56</v>
       </c>
-      <c r="N29" s="152">
+      <c r="N29" s="150">
         <f>(N26*1000000)/3600000</f>
         <v>21.503333333333337</v>
       </c>
@@ -3377,23 +3602,23 @@
     <row r="30" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B30" s="103"/>
       <c r="C30" s="104"/>
-      <c r="M30" s="149"/>
-      <c r="N30" s="153"/>
+      <c r="M30" s="147"/>
+      <c r="N30" s="151"/>
     </row>
     <row r="31" spans="2:16" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="103"/>
       <c r="C31" s="104"/>
-      <c r="M31" s="150" t="s">
+      <c r="M31" s="148" t="s">
         <v>58</v>
       </c>
-      <c r="N31" s="152">
+      <c r="N31" s="150">
         <f>N29*C19</f>
         <v>4.3006666666666673</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="M32" s="151"/>
-      <c r="N32" s="153"/>
+      <c r="M32" s="149"/>
+      <c r="N32" s="151"/>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.35">
       <c r="C33"/>
@@ -3567,12 +3792,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="F16:F18"/>
-    <mergeCell ref="F19:F21"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="N22:N24"/>
-    <mergeCell ref="N16:N18"/>
-    <mergeCell ref="N19:N21"/>
     <mergeCell ref="M29:M30"/>
     <mergeCell ref="M31:M32"/>
     <mergeCell ref="N29:N30"/>
@@ -3583,6 +3802,12 @@
     <mergeCell ref="N10:N12"/>
     <mergeCell ref="N13:N15"/>
     <mergeCell ref="F13:F15"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="N22:N24"/>
+    <mergeCell ref="N16:N18"/>
+    <mergeCell ref="N19:N21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3594,373 +3819,897 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF1D9A0-CB34-4E78-B9E9-B31733748EC3}">
-  <dimension ref="B6:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54DE5658-1F6B-4037-8C75-503501F26DA5}">
+  <dimension ref="B2:F83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.90625" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" customWidth="1"/>
-    <col min="7" max="7" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="120" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="120" t="s">
-        <v>66</v>
-      </c>
-      <c r="H6" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F2" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="114"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="117" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="86">
         <v>9.81</v>
       </c>
-      <c r="E7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F7" t="s">
-        <v>95</v>
-      </c>
-      <c r="H7" s="141">
-        <f>(0.5*C8*C9*12*2*C7*65)/1000000</f>
-        <v>12.013326000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8">
+      <c r="E7" s="107" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="143">
+        <f>(0.5*C$12*SQRT(2*C$7*C$14*74)^2)/1000000</f>
+        <v>64.554069311999996</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="88" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="89">
+        <v>314</v>
+      </c>
+      <c r="E8" s="107" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="143">
+        <f>(0.5*C$12*SQRT(2*C$7*C$14*60)^2)/1000000</f>
+        <v>52.341137279999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="88" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="89">
         <v>1000</v>
       </c>
-      <c r="E8" t="s">
-        <v>85</v>
-      </c>
-      <c r="F8" t="s">
-        <v>93</v>
-      </c>
-      <c r="H8" s="141">
-        <f>(0.5*C8*C9*12*2*C7*130)/1000000</f>
-        <v>24.026652000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9">
-        <v>1.57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>86</v>
-      </c>
-      <c r="F9" t="s">
-        <v>94</v>
-      </c>
-      <c r="H9" s="141">
-        <f>(0.5*C8*C9*12*2*C7*195)/1000000</f>
-        <v>36.039978000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10">
+      <c r="E9" s="107" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="143">
+        <f>(0.5*C$12*SQRT(2*C$7*C$14*46)^2)/1000000</f>
+        <v>40.128205247999993</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="89">
+        <v>5</v>
+      </c>
+      <c r="E10" s="107" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="143">
+        <f>(0.5*C$12*SQRT(2*C$7*C$14*32)^2)/1000000</f>
+        <v>27.915273215999999</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="88" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="89">
+        <f>C8*C10</f>
+        <v>1570</v>
+      </c>
+      <c r="E11" s="107" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="143">
+        <f>(0.5*C$12*SQRT(2*C$7*C$14*18)^2)/1000000</f>
+        <v>15.702341183999996</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="123">
+        <f>C11*12</f>
+        <v>18840</v>
+      </c>
+      <c r="E12" s="109" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="123">
+        <f>C11*16</f>
+        <v>25120</v>
+      </c>
+      <c r="E13" s="164" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="142">
+        <f>F7+F8+F9+F10+F11+F12</f>
+        <v>200.64102624</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="125" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="86">
         <v>4.72</v>
       </c>
-      <c r="E10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" t="s">
-        <v>96</v>
-      </c>
-      <c r="H10" s="141">
-        <f>(0.5*C8*C9*12*2*C7*260)/1000000</f>
-        <v>48.053304000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11">
+      <c r="E14" s="165" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="160">
+        <f>F13*C17</f>
+        <v>160.512820992</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="124" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="89">
+        <v>16</v>
+      </c>
+      <c r="E15" s="166"/>
+      <c r="F15" s="160"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="88" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="89">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="125" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="86">
         <v>0.8</v>
       </c>
-      <c r="E11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="141">
-        <f>(0.5*C8*C9*12*2*C7*325)/1000000</f>
-        <v>60.066630000000011</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12">
-        <v>0.9</v>
-      </c>
-      <c r="G12" t="s">
-        <v>52</v>
-      </c>
-      <c r="H12" s="141">
-        <f>H7+H8+H9+H10+H11</f>
-        <v>180.19989000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>0.1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>90</v>
-      </c>
-      <c r="H13" s="141">
-        <f>H12*C11*C12</f>
-        <v>129.74392080000001</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="121">
-        <v>86400</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15">
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="126" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="85">
+        <v>9.44</v>
+      </c>
+      <c r="E18" s="146" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="162">
+        <f>(F14*1000000)/3600000</f>
+        <v>44.586894720000004</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="126" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="85">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="G16" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="141">
-        <f>H13/3.6</f>
-        <v>36.039978000000005</v>
-      </c>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H17" s="18">
-        <f>H16*C15</f>
-        <v>7.2079956000000012</v>
-      </c>
+      <c r="E19" s="147"/>
+      <c r="F19" s="162"/>
+    </row>
+    <row r="20" spans="2:6" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="115"/>
+      <c r="C20" s="116"/>
+      <c r="E20" s="167" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="162">
+        <f>F18*C19</f>
+        <v>8.9173789440000011</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="139"/>
+      <c r="C21" s="112"/>
+      <c r="E21" s="168"/>
+      <c r="F21" s="162"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="103"/>
+      <c r="C22" s="104"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="96"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F23" s="95"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F24" s="95"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="95"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F26" s="110"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="103"/>
+      <c r="F27" s="95"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="103"/>
+      <c r="C28" s="104"/>
+      <c r="F28" s="95"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="103"/>
+      <c r="C29" s="104"/>
+      <c r="F29" s="95"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="103"/>
+      <c r="C30" s="104"/>
+      <c r="F30" s="95"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="103"/>
+      <c r="C31" s="104"/>
+      <c r="F31" s="95"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F32" s="95"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C33"/>
+      <c r="F33" s="95"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C34"/>
+      <c r="F34" s="95"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C35"/>
+      <c r="F35" s="95"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C36"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C37"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C38"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C39"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C40"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C41"/>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C42"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C43"/>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C44"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C45"/>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C46"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C47"/>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C48"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C49"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C50"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C51"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C52"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C53"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C54"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C55"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C56"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C57"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C58"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C59"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C60"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C61"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C62"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C63"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C64"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C65"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C66"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C67"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C68"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C69"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C70"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C71"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C72"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C73"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C74"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C75"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C76"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C77"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C78"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C79"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C80"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C81"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C82"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C83"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F20:F21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40C3B2D-E4BE-4431-A41F-5268AC320356}">
-  <dimension ref="B6:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214539A3-4734-4BA8-9E72-FADCFDFC14E2}">
+  <dimension ref="B2:F83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView showGridLines="0" topLeftCell="D7" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="24.7265625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="8" max="8" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="26.1796875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" customWidth="1"/>
+    <col min="6" max="6" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="120" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="120" t="s">
-        <v>66</v>
-      </c>
-      <c r="I6" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F2" s="18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B6" s="113" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="114"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="117" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="86">
         <v>9.81</v>
       </c>
-      <c r="E7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" t="s">
-        <v>103</v>
-      </c>
-      <c r="I7" s="141">
-        <f>(12*C9*C8*C7*65*(1+C11)^0)/1000000</f>
-        <v>12.013326000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8">
+      <c r="E7" s="107" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="143">
+        <f>(0.5*C$12*SQRT(2*C$7*C$14*13)^2)/1000000</f>
+        <v>11.340579743999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="88" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="89">
+        <v>314</v>
+      </c>
+      <c r="E8" s="107" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="143">
+        <f>(0.5*2*C$12*SQRT(2*C$7*C$14*13)^2)/1000000</f>
+        <v>22.681159487999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B9" s="88" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="89">
         <v>1000</v>
       </c>
-      <c r="E8" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" t="s">
-        <v>104</v>
-      </c>
-      <c r="I8" s="141">
-        <f>(12*C9*C8*C7*65*(1+C11)^1)/1000000</f>
-        <v>21.623986800000004</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C9">
-        <v>1.57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" t="s">
-        <v>105</v>
-      </c>
-      <c r="I9" s="141">
-        <f>(12*C9*C8*C7*65*(1+C11)^2)/1000000</f>
-        <v>38.923176240000011</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10">
+      <c r="E9" s="107" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="143">
+        <f>(0.5*3*C$12*SQRT(2*C$7*C$14*13)^2)/1000000</f>
+        <v>34.021739232000002</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B10" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="89">
+        <v>5</v>
+      </c>
+      <c r="E10" s="107" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="143">
+        <f>(0.5*4*C$12*SQRT(2*C$7*C$14*13)^2)/1000000</f>
+        <v>45.362318975999997</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B11" s="88" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="89">
+        <f>C8*C10</f>
+        <v>1570</v>
+      </c>
+      <c r="E11" s="107" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="143">
+        <f>(0.5*5*C$12*SQRT(2*C$7*C$14*18)^2)/1000000</f>
+        <v>78.511705919999983</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="123">
+        <f>C11*12</f>
+        <v>18840</v>
+      </c>
+      <c r="E12" s="109" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B13" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="123">
+        <f>C11*16</f>
+        <v>25120</v>
+      </c>
+      <c r="E13" s="164" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="142">
+        <f>F7+F8+F9+F10+F11+F12</f>
+        <v>191.91750335999998</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="125" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="86">
         <v>4.72</v>
       </c>
-      <c r="E10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" t="s">
-        <v>106</v>
-      </c>
-      <c r="I10" s="141">
-        <f>(12*C9*C8*C7*65*(1+C11)^3)/1000000</f>
-        <v>70.061717232000021</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11">
+      <c r="E14" s="165" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="160">
+        <f>F13*C17</f>
+        <v>153.53400268799999</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B15" s="124" t="s">
+        <v>109</v>
+      </c>
+      <c r="C15" s="89">
+        <v>16</v>
+      </c>
+      <c r="E15" s="166"/>
+      <c r="F15" s="160"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B16" s="88" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="89">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" s="125" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="86">
         <v>0.8</v>
       </c>
-      <c r="E11" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" t="s">
-        <v>107</v>
-      </c>
-      <c r="I11" s="141">
-        <f>(12*C9*C8*C7*65*(1+C11)^4)/1000000</f>
-        <v>126.11109101760005</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12">
-        <v>0.9</v>
-      </c>
-      <c r="H12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I12" s="141">
-        <f>I7+I8+I9+I10+I11</f>
-        <v>268.73329728960005</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>0.1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>90</v>
-      </c>
-      <c r="I13" s="141">
-        <f>I12*C11*C12</f>
-        <v>193.48797404851203</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="121">
-        <v>86400</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15">
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="126" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="85">
+        <v>9.44</v>
+      </c>
+      <c r="E18" s="146" t="s">
+        <v>56</v>
+      </c>
+      <c r="F18" s="162">
+        <f>(F14*1000000)/3600000</f>
+        <v>42.648334079999998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="126" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="85">
         <v>0.2</v>
       </c>
-      <c r="H15" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15">
-        <f>I13/3.6</f>
-        <v>53.746659457920003</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="H16" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16">
-        <f>I15*C15</f>
-        <v>10.749331891584001</v>
-      </c>
+      <c r="E19" s="147"/>
+      <c r="F19" s="162"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" s="115"/>
+      <c r="C20" s="116"/>
+      <c r="E20" s="167" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="162">
+        <f>F18*C19</f>
+        <v>8.5296668160000007</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B21" s="139"/>
+      <c r="C21" s="112"/>
+      <c r="E21" s="168"/>
+      <c r="F21" s="162"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" s="103"/>
+      <c r="C22" s="104"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="96"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F23" s="95"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F24" s="95"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F25" s="95"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F26" s="110"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="103"/>
+      <c r="F27" s="95"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="103"/>
+      <c r="C28" s="104"/>
+      <c r="F28" s="95"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="103"/>
+      <c r="C29" s="104"/>
+      <c r="F29" s="95"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="103"/>
+      <c r="C30" s="104"/>
+      <c r="F30" s="95"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="103"/>
+      <c r="C31" s="104"/>
+      <c r="F31" s="95"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F32" s="95"/>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C33"/>
+      <c r="F33" s="95"/>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C34"/>
+      <c r="F34" s="95"/>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C35"/>
+      <c r="F35" s="95"/>
+    </row>
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C36"/>
+    </row>
+    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C37"/>
+    </row>
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C38"/>
+    </row>
+    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C39"/>
+    </row>
+    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C40"/>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C41"/>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C42"/>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C43"/>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C44"/>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C45"/>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C46"/>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C47"/>
+    </row>
+    <row r="48" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C48"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C49"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C50"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C51"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C52"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C53"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C54"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C55"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C56"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C57"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C58"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C59"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C60"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C61"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C62"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C63"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C64"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C65"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C66"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C67"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C68"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C69"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C70"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C71"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C72"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C73"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C74"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C75"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C76"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C77"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C78"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C79"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C80"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C81"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C82"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C83"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -3969,7 +4718,7 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20:N21"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4070,7 +4819,7 @@
         <v>9.81</v>
       </c>
       <c r="F7" s="19"/>
-      <c r="G7" s="154" t="s">
+      <c r="G7" s="156" t="s">
         <v>37</v>
       </c>
       <c r="H7" s="97">
@@ -4078,7 +4827,7 @@
         <v>0.94504831200000006</v>
       </c>
       <c r="I7" s="91"/>
-      <c r="J7" s="154" t="s">
+      <c r="J7" s="156" t="s">
         <v>38</v>
       </c>
       <c r="K7" s="97">
@@ -4104,13 +4853,13 @@
         <v>314</v>
       </c>
       <c r="F8" s="19"/>
-      <c r="G8" s="155"/>
+      <c r="G8" s="157"/>
       <c r="H8" s="97">
         <f t="shared" si="0"/>
         <v>0.87235228800000009</v>
       </c>
       <c r="I8" s="91"/>
-      <c r="J8" s="155"/>
+      <c r="J8" s="157"/>
       <c r="K8" s="97">
         <f t="shared" si="1"/>
         <v>1.0904403600000001</v>
@@ -4134,13 +4883,13 @@
         <v>1000</v>
       </c>
       <c r="F9" s="19"/>
-      <c r="G9" s="155"/>
+      <c r="G9" s="157"/>
       <c r="H9" s="97">
         <f t="shared" si="0"/>
         <v>0.79965626400000012</v>
       </c>
       <c r="I9" s="91"/>
-      <c r="J9" s="155"/>
+      <c r="J9" s="157"/>
       <c r="K9" s="97">
         <f t="shared" si="1"/>
         <v>1.017744336</v>
@@ -4164,13 +4913,13 @@
         <v>5</v>
       </c>
       <c r="F10" s="19"/>
-      <c r="G10" s="155"/>
+      <c r="G10" s="157"/>
       <c r="H10" s="97">
         <f t="shared" si="0"/>
         <v>0.72696024000000015</v>
       </c>
       <c r="I10" s="94"/>
-      <c r="J10" s="155"/>
+      <c r="J10" s="157"/>
       <c r="K10" s="97">
         <f t="shared" si="1"/>
         <v>0.94504831200000006</v>
@@ -4191,13 +4940,13 @@
       <c r="E11" s="86">
         <v>4.72</v>
       </c>
-      <c r="G11" s="155"/>
+      <c r="G11" s="157"/>
       <c r="H11" s="97">
         <f t="shared" si="0"/>
         <v>0.65426421600000018</v>
       </c>
       <c r="I11" s="91"/>
-      <c r="J11" s="155"/>
+      <c r="J11" s="157"/>
       <c r="K11" s="97">
         <f t="shared" si="1"/>
         <v>0.87235228800000009</v>
@@ -4221,13 +4970,13 @@
         <v>0.8</v>
       </c>
       <c r="F12" s="19"/>
-      <c r="G12" s="155"/>
+      <c r="G12" s="157"/>
       <c r="H12" s="97">
         <f t="shared" si="0"/>
         <v>0.58156819199999998</v>
       </c>
       <c r="I12" s="91"/>
-      <c r="J12" s="155"/>
+      <c r="J12" s="157"/>
       <c r="K12" s="97">
         <f t="shared" si="1"/>
         <v>0.79965626400000001</v>
@@ -4251,13 +5000,13 @@
         <v>66.08</v>
       </c>
       <c r="F13" s="91"/>
-      <c r="G13" s="155"/>
+      <c r="G13" s="157"/>
       <c r="H13" s="97">
         <f t="shared" si="0"/>
         <v>0.50887216800000001</v>
       </c>
       <c r="I13" s="91"/>
-      <c r="J13" s="155"/>
+      <c r="J13" s="157"/>
       <c r="K13" s="97">
         <f t="shared" si="1"/>
         <v>0.72696024000000004</v>
@@ -4281,22 +5030,22 @@
         <v>80.239999999999995</v>
       </c>
       <c r="F14" s="91"/>
-      <c r="G14" s="155"/>
+      <c r="G14" s="157"/>
       <c r="H14" s="97">
         <f t="shared" si="0"/>
         <v>0.43617614400000004</v>
       </c>
       <c r="I14" s="91"/>
-      <c r="J14" s="155"/>
+      <c r="J14" s="157"/>
       <c r="K14" s="97">
         <f t="shared" si="1"/>
         <v>0.65426421600000007</v>
       </c>
       <c r="L14" s="18"/>
-      <c r="M14" s="157" t="s">
+      <c r="M14" s="159" t="s">
         <v>54</v>
       </c>
-      <c r="N14" s="158">
+      <c r="N14" s="160">
         <f>N13*E12</f>
         <v>191.10330789120005</v>
       </c>
@@ -4312,20 +5061,20 @@
         <v>410.64</v>
       </c>
       <c r="F15" s="91"/>
-      <c r="G15" s="155"/>
+      <c r="G15" s="157"/>
       <c r="H15" s="97">
         <f t="shared" si="0"/>
         <v>0.36348012000000007</v>
       </c>
       <c r="I15" s="91"/>
-      <c r="J15" s="155"/>
+      <c r="J15" s="157"/>
       <c r="K15" s="97">
         <f t="shared" si="1"/>
         <v>0.58156819199999998</v>
       </c>
       <c r="L15" s="18"/>
-      <c r="M15" s="157"/>
-      <c r="N15" s="158"/>
+      <c r="M15" s="159"/>
+      <c r="N15" s="160"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="92"/>
@@ -4337,13 +5086,13 @@
         <v>0.2</v>
       </c>
       <c r="F16" s="91"/>
-      <c r="G16" s="155"/>
+      <c r="G16" s="157"/>
       <c r="H16" s="97">
         <f t="shared" si="0"/>
         <v>0.2907840960000001</v>
       </c>
       <c r="I16" s="94"/>
-      <c r="J16" s="155"/>
+      <c r="J16" s="157"/>
       <c r="K16" s="97">
         <f t="shared" si="1"/>
         <v>0.50887216800000001</v>
@@ -4356,13 +5105,13 @@
       <c r="D17" s="115"/>
       <c r="E17" s="116"/>
       <c r="F17" s="91"/>
-      <c r="G17" s="155"/>
+      <c r="G17" s="157"/>
       <c r="H17" s="97">
         <f t="shared" si="0"/>
         <v>0.21808807200000008</v>
       </c>
       <c r="I17" s="91"/>
-      <c r="J17" s="155"/>
+      <c r="J17" s="157"/>
       <c r="K17" s="97">
         <f t="shared" si="1"/>
         <v>0.43617614400000004</v>
@@ -4375,22 +5124,22 @@
       <c r="D18" s="111"/>
       <c r="E18" s="112"/>
       <c r="F18" s="91"/>
-      <c r="G18" s="156"/>
+      <c r="G18" s="158"/>
       <c r="H18" s="106">
         <f t="shared" si="0"/>
         <v>0.14539204799999997</v>
       </c>
       <c r="I18" s="91"/>
-      <c r="J18" s="155"/>
+      <c r="J18" s="157"/>
       <c r="K18" s="102">
         <f t="shared" si="1"/>
         <v>0.36348011999999996</v>
       </c>
       <c r="L18" s="18"/>
-      <c r="M18" s="159" t="s">
+      <c r="M18" s="161" t="s">
         <v>56</v>
       </c>
-      <c r="N18" s="160">
+      <c r="N18" s="162">
         <f>(N14*1000000)/3600000</f>
         <v>53.084252192000008</v>
       </c>
@@ -4409,14 +5158,14 @@
         <v>6.5426421600000015</v>
       </c>
       <c r="I19" s="18"/>
-      <c r="J19" s="155"/>
+      <c r="J19" s="157"/>
       <c r="K19" s="102">
         <f t="shared" si="1"/>
         <v>0.29078409599999994</v>
       </c>
       <c r="L19" s="18"/>
-      <c r="M19" s="159"/>
-      <c r="N19" s="160"/>
+      <c r="M19" s="161"/>
+      <c r="N19" s="162"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B20" s="92"/>
@@ -4425,16 +5174,16 @@
       <c r="E20" s="112"/>
       <c r="F20" s="91"/>
       <c r="I20" s="18"/>
-      <c r="J20" s="155"/>
+      <c r="J20" s="157"/>
       <c r="K20" s="102">
         <f t="shared" si="1"/>
         <v>0.21808807199999997</v>
       </c>
       <c r="L20" s="18"/>
-      <c r="M20" s="161" t="s">
+      <c r="M20" s="163" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="160">
+      <c r="N20" s="162">
         <f>N18*E16</f>
         <v>10.616850438400002</v>
       </c>
@@ -4446,14 +5195,14 @@
       <c r="E21" s="112"/>
       <c r="F21" s="91"/>
       <c r="I21" s="18"/>
-      <c r="J21" s="155"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="102">
         <f t="shared" si="1"/>
         <v>0.14539204799999997</v>
       </c>
       <c r="L21" s="18"/>
-      <c r="M21" s="161"/>
-      <c r="N21" s="160"/>
+      <c r="M21" s="163"/>
+      <c r="N21" s="162"/>
     </row>
     <row r="22" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="93"/>
@@ -4464,7 +5213,7 @@
       <c r="G22" s="18"/>
       <c r="H22" s="96"/>
       <c r="I22" s="18"/>
-      <c r="J22" s="156"/>
+      <c r="J22" s="158"/>
       <c r="K22" s="106">
         <f t="shared" si="1"/>
         <v>7.2696023999999984E-2</v>
@@ -4669,4 +5418,375 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40C3B2D-E4BE-4431-A41F-5268AC320356}">
+  <dimension ref="B6:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B6" s="120" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="120" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>9.81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" t="s">
+        <v>103</v>
+      </c>
+      <c r="I7" s="141">
+        <f>(12*C9*C8*C7*65*(1+C11)^0)/1000000</f>
+        <v>12.013326000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8">
+        <v>1000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" s="141">
+        <f>(12*C9*C8*C7*65*(1+C11)^1)/1000000</f>
+        <v>21.623986800000004</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <v>1.57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="141">
+        <f>(12*C9*C8*C7*65*(1+C11)^2)/1000000</f>
+        <v>38.923176240000011</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10">
+        <v>4.72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I10" s="141">
+        <f>(12*C9*C8*C7*65*(1+C11)^3)/1000000</f>
+        <v>70.061717232000021</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11">
+        <v>0.8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="141">
+        <f>(12*C9*C8*C7*65*(1+C11)^4)/1000000</f>
+        <v>126.11109101760005</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12">
+        <v>0.9</v>
+      </c>
+      <c r="H12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I12" s="141">
+        <f>I7+I8+I9+I10+I11</f>
+        <v>268.73329728960005</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>0.1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="141">
+        <f>I12*C11*C12</f>
+        <v>193.48797404851203</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="121">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15">
+        <v>0.2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15">
+        <f>I13/3.6</f>
+        <v>53.746659457920003</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16">
+        <f>I15*C15</f>
+        <v>10.749331891584001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF1D9A0-CB34-4E78-B9E9-B31733748EC3}">
+  <dimension ref="B6:H17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="24.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="120" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="120" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7">
+        <v>9.81</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="141">
+        <f>(0.5*C8*C9*12*2*C7*65)/1000000</f>
+        <v>12.013326000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8">
+        <v>1000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="141">
+        <f>(0.5*C8*C9*12*2*C7*130)/1000000</f>
+        <v>24.026652000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9">
+        <v>1.57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="141">
+        <f>(0.5*C8*C9*12*2*C7*195)/1000000</f>
+        <v>36.039978000000005</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10">
+        <v>4.72</v>
+      </c>
+      <c r="E10" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H10" s="141">
+        <f>(0.5*C8*C9*12*2*C7*260)/1000000</f>
+        <v>48.053304000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11">
+        <v>0.8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H11" s="141">
+        <f>(0.5*C8*C9*12*2*C7*325)/1000000</f>
+        <v>60.066630000000011</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12">
+        <v>0.9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>52</v>
+      </c>
+      <c r="H12" s="141">
+        <f>H7+H8+H9+H10+H11</f>
+        <v>180.19989000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>0.1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="141">
+        <f>H12*C11*C12</f>
+        <v>129.74392080000001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="121">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="141">
+        <f>H13/3.6</f>
+        <v>36.039978000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="18">
+        <f>H16*C15</f>
+        <v>7.2079956000000012</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>